<commit_message>
default calculation of decharge curve added
</commit_message>
<xml_diff>
--- a/software/BikeCounterPro/src/dataPackage/DataPackage.xlsx
+++ b/software/BikeCounterPro/src/dataPackage/DataPackage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meier\Documents\repos\bikecounter\hardware\BikeCounterPro\src\dataPackage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meier\Documents\repos\bikecounter\software\BikeCounterPro\src\dataPackage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEA4BA4-A91E-4B05-98FD-EB6F6FE6D292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF565487-F116-482D-8164-61885B025632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9312" yWindow="3180" windowWidth="31968" windowHeight="13500" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" activeTab="3" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Data package" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="127">
   <si>
     <t>minutes of day</t>
   </si>
@@ -392,6 +392,33 @@
   </si>
   <si>
     <t>d11abf00db12795104943221308b7b15bbd1c374 [d11abf0]</t>
+  </si>
+  <si>
+    <t>Volateg</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>a0</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>a2</t>
+  </si>
+  <si>
+    <t>a3</t>
+  </si>
+  <si>
+    <t>a4</t>
+  </si>
+  <si>
+    <t>a5</t>
+  </si>
+  <si>
+    <t>calc</t>
   </si>
 </sst>
 </file>
@@ -654,21 +681,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -697,9 +727,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -756,6 +783,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-CH"/>
+              <a:t>Version 1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1264,7 +1316,955 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Version 2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CH"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18122464461730509"/>
+          <c:y val="0.11073522734521875"/>
+          <c:w val="0.76013226836200043"/>
+          <c:h val="0.83151559726667879"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BatteryVotage!$B$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="5"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.14469703454175978"/>
+                  <c:y val="-6.6891016139502948E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.0000000000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-CH"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>BatteryVotage!$A$31:$A$63</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.05</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.95</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.85</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.65</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.55</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.45</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.35</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.15</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.05</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.95</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.85</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.7500000000000102</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.7000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.6500000000000101</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.6000000000000099</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>BatteryVotage!$B$31:$B$63</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>99.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C566-4B14-880B-DE055377ED1C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>calc</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>BatteryVotage!$A$31:$A$55</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.05</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.95</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.85</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.65</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.55</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.45</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.35</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.15</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.05</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>BatteryVotage!$C$31:$C$55</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>100.04675371996564</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>99.405541643900506</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97.885026838273916</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95.511479702858196</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>92.330696823737526</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>88.405632938047347</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>83.814032900780148</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>78.646063650106953</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>73.001946173659235</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>66.989587474461587</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60.722212536311417</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>54.315996290177281</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>47.887695580277068</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41.55228112925397</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>35.420569505040476</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>29.596855085597781</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24.176542026129027</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19.243776223993336</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14.869077284987725</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11.106970489425294</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.9936187574858195</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.5444546161379549</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.7518121635876014</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.5825590366948745</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.9757283759172424</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C566-4B14-880B-DE055377ED1C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="637611535"/>
+        <c:axId val="770739263"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="637611535"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="4.5"/>
+          <c:min val="2.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-CH"/>
+                  <a:t>Voltage</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-CH"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="770739263"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="770739263"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="-3"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-CH"/>
+                  <a:t>%</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-CH"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="637611535"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-CH"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1820,20 +2820,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>116681</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:colOff>177641</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>20002</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>116681</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>177641</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>34290</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1853,6 +3369,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>196361</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>26963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>51581</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>147711</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E5CDC41-5519-9B20-729D-5CBBE2F2C98B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2160,7 +3712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088FF0E6-8FE4-49E3-812F-B76B934E1ACD}">
   <dimension ref="A1:S90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -3231,46 +4783,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="26" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="26" t="s">
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="26" t="s">
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="29"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
@@ -3371,52 +4923,52 @@
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="32" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="32" t="s">
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="O3" s="33"/>
-      <c r="P3" s="34"/>
-      <c r="Q3" s="32" t="s">
+      <c r="O3" s="34"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="R3" s="33"/>
-      <c r="S3" s="34"/>
-      <c r="T3" s="29" t="s">
+      <c r="R3" s="34"/>
+      <c r="S3" s="35"/>
+      <c r="T3" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="U3" s="30"/>
-      <c r="V3" s="30"/>
-      <c r="W3" s="30"/>
-      <c r="X3" s="31"/>
-      <c r="Y3" s="29" t="s">
+      <c r="U3" s="31"/>
+      <c r="V3" s="31"/>
+      <c r="W3" s="31"/>
+      <c r="X3" s="32"/>
+      <c r="Y3" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="30"/>
-      <c r="AA3" s="30"/>
-      <c r="AB3" s="30"/>
-      <c r="AC3" s="31"/>
-      <c r="AD3" s="29" t="s">
+      <c r="Z3" s="31"/>
+      <c r="AA3" s="31"/>
+      <c r="AB3" s="31"/>
+      <c r="AC3" s="32"/>
+      <c r="AD3" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="AE3" s="30"/>
-      <c r="AF3" s="31"/>
+      <c r="AE3" s="31"/>
+      <c r="AF3" s="32"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
@@ -3476,46 +5028,46 @@
       <c r="AF5" s="25"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24">
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26">
         <v>38</v>
       </c>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24">
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26">
         <v>73</v>
       </c>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
-      <c r="T6" s="24"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="24"/>
-      <c r="W6" s="24"/>
-      <c r="X6" s="24"/>
-      <c r="Y6" s="24">
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="26"/>
+      <c r="W6" s="26"/>
+      <c r="X6" s="26"/>
+      <c r="Y6" s="26">
         <v>88</v>
       </c>
-      <c r="Z6" s="24"/>
-      <c r="AA6" s="24"/>
-      <c r="AB6" s="24"/>
-      <c r="AC6" s="24"/>
-      <c r="AD6" s="24"/>
-      <c r="AE6" s="24"/>
-      <c r="AF6" s="24"/>
+      <c r="Z6" s="26"/>
+      <c r="AA6" s="26"/>
+      <c r="AB6" s="26"/>
+      <c r="AC6" s="26"/>
+      <c r="AD6" s="26"/>
+      <c r="AE6" s="26"/>
+      <c r="AF6" s="26"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
@@ -3616,203 +5168,203 @@
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20" t="s">
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="20" t="s">
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="R8" s="20"/>
-      <c r="S8" s="20"/>
-      <c r="T8" s="20" t="s">
+      <c r="R8" s="22"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="U8" s="20"/>
-      <c r="V8" s="20"/>
-      <c r="W8" s="20"/>
-      <c r="X8" s="20"/>
-      <c r="Y8" s="20" t="s">
+      <c r="U8" s="22"/>
+      <c r="V8" s="22"/>
+      <c r="W8" s="22"/>
+      <c r="X8" s="22"/>
+      <c r="Y8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="Z8" s="20"/>
-      <c r="AA8" s="20"/>
-      <c r="AB8" s="20"/>
-      <c r="AC8" s="20"/>
-      <c r="AD8" s="20" t="s">
+      <c r="Z8" s="22"/>
+      <c r="AA8" s="22"/>
+      <c r="AB8" s="22"/>
+      <c r="AC8" s="22"/>
+      <c r="AD8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="AE8" s="20"/>
-      <c r="AF8" s="20"/>
+      <c r="AE8" s="22"/>
+      <c r="AF8" s="22"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A9" s="20">
+      <c r="A9" s="22">
         <v>10</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20">
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22">
         <v>7</v>
       </c>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20">
-        <v>0</v>
-      </c>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="20">
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22">
+        <v>0</v>
+      </c>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22">
         <v>3</v>
       </c>
-      <c r="R9" s="20"/>
-      <c r="S9" s="20"/>
-      <c r="T9" s="20">
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22">
         <v>19</v>
       </c>
-      <c r="U9" s="20"/>
-      <c r="V9" s="20"/>
-      <c r="W9" s="20"/>
-      <c r="X9" s="20"/>
-      <c r="Y9" s="20">
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22">
         <v>17</v>
       </c>
-      <c r="Z9" s="20"/>
-      <c r="AA9" s="20"/>
-      <c r="AB9" s="20"/>
-      <c r="AC9" s="20"/>
-      <c r="AD9" s="20">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="20"/>
-      <c r="AF9" s="20"/>
+      <c r="Z9" s="22"/>
+      <c r="AA9" s="22"/>
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="22"/>
+      <c r="AD9" s="22">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="22"/>
+      <c r="AF9" s="22"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20" t="s">
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20" t="s">
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="R10" s="20"/>
-      <c r="S10" s="20"/>
-      <c r="T10" s="20" t="s">
+      <c r="R10" s="22"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="U10" s="20"/>
-      <c r="V10" s="20"/>
-      <c r="W10" s="20"/>
-      <c r="X10" s="20"/>
-      <c r="Y10" s="20" t="s">
+      <c r="U10" s="22"/>
+      <c r="V10" s="22"/>
+      <c r="W10" s="22"/>
+      <c r="X10" s="22"/>
+      <c r="Y10" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="Z10" s="20"/>
-      <c r="AA10" s="20"/>
-      <c r="AB10" s="20"/>
-      <c r="AC10" s="20"/>
-      <c r="AD10" s="20" t="s">
+      <c r="Z10" s="22"/>
+      <c r="AA10" s="22"/>
+      <c r="AB10" s="22"/>
+      <c r="AC10" s="22"/>
+      <c r="AD10" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="AE10" s="20"/>
-      <c r="AF10" s="20"/>
+      <c r="AE10" s="22"/>
+      <c r="AF10" s="22"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A11" s="20">
+      <c r="A11" s="22">
         <f>A9</f>
         <v>10</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="21">
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="23">
         <f>'Data package'!$B$31*I9+'Data package'!$B$28</f>
         <v>3.338709677419355</v>
       </c>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="22">
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="20">
         <f ca="1">LOOKUP(N9,'Data package'!$D$21:$D$24,'Data package'!$E$22:$E$35)</f>
         <v>0</v>
       </c>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="23">
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="24">
         <f>100/(2^3-1)*Q9</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23">
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24">
         <f>'Data package'!$B$40*T9+'Data package'!$B$37</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U11" s="22"/>
-      <c r="V11" s="22"/>
-      <c r="W11" s="22"/>
-      <c r="X11" s="22"/>
-      <c r="Y11" s="22">
+      <c r="U11" s="20"/>
+      <c r="V11" s="20"/>
+      <c r="W11" s="20"/>
+      <c r="X11" s="20"/>
+      <c r="Y11" s="20">
         <f>Y9</f>
         <v>17</v>
       </c>
-      <c r="Z11" s="22"/>
-      <c r="AA11" s="22"/>
-      <c r="AB11" s="22"/>
-      <c r="AC11" s="22"/>
-      <c r="AD11" s="22">
+      <c r="Z11" s="20"/>
+      <c r="AA11" s="20"/>
+      <c r="AB11" s="20"/>
+      <c r="AC11" s="20"/>
+      <c r="AD11" s="20">
         <f>LOOKUP(AD9,'Data package'!$A$84:$A$88,'Data package'!$B$84:$B$88)</f>
         <v>1</v>
       </c>
-      <c r="AE11" s="22"/>
-      <c r="AF11" s="22"/>
+      <c r="AE11" s="20"/>
+      <c r="AF11" s="20"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
@@ -3864,46 +5416,46 @@
       <c r="AF14" s="25"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24" t="s">
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24" t="s">
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
-      <c r="U15" s="24"/>
-      <c r="V15" s="24"/>
-      <c r="W15" s="24"/>
-      <c r="X15" s="24"/>
-      <c r="Y15" s="24" t="s">
+      <c r="R15" s="26"/>
+      <c r="S15" s="26"/>
+      <c r="T15" s="26"/>
+      <c r="U15" s="26"/>
+      <c r="V15" s="26"/>
+      <c r="W15" s="26"/>
+      <c r="X15" s="26"/>
+      <c r="Y15" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="Z15" s="24"/>
-      <c r="AA15" s="24"/>
-      <c r="AB15" s="24"/>
-      <c r="AC15" s="24"/>
-      <c r="AD15" s="24"/>
-      <c r="AE15" s="24"/>
-      <c r="AF15" s="24"/>
+      <c r="Z15" s="26"/>
+      <c r="AA15" s="26"/>
+      <c r="AB15" s="26"/>
+      <c r="AC15" s="26"/>
+      <c r="AD15" s="26"/>
+      <c r="AE15" s="26"/>
+      <c r="AF15" s="26"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
@@ -4004,203 +5556,203 @@
       </c>
     </row>
     <row r="17" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20" t="s">
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="20" t="s">
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="O17" s="20"/>
-      <c r="P17" s="20"/>
-      <c r="Q17" s="20" t="s">
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="R17" s="20"/>
-      <c r="S17" s="20"/>
-      <c r="T17" s="20" t="s">
+      <c r="R17" s="22"/>
+      <c r="S17" s="22"/>
+      <c r="T17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="U17" s="20"/>
-      <c r="V17" s="20"/>
-      <c r="W17" s="20"/>
-      <c r="X17" s="20"/>
-      <c r="Y17" s="20" t="s">
+      <c r="U17" s="22"/>
+      <c r="V17" s="22"/>
+      <c r="W17" s="22"/>
+      <c r="X17" s="22"/>
+      <c r="Y17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="Z17" s="20"/>
-      <c r="AA17" s="20"/>
-      <c r="AB17" s="20"/>
-      <c r="AC17" s="20"/>
-      <c r="AD17" s="20" t="s">
+      <c r="Z17" s="22"/>
+      <c r="AA17" s="22"/>
+      <c r="AB17" s="22"/>
+      <c r="AC17" s="22"/>
+      <c r="AD17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="AE17" s="20"/>
-      <c r="AF17" s="20"/>
+      <c r="AE17" s="22"/>
+      <c r="AF17" s="22"/>
     </row>
     <row r="18" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A18" s="20">
+      <c r="A18" s="22">
         <v>5</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20">
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22">
         <v>8</v>
       </c>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20">
-        <v>0</v>
-      </c>
-      <c r="O18" s="20"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="20">
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22">
+        <v>0</v>
+      </c>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22">
         <v>3</v>
       </c>
-      <c r="R18" s="20"/>
-      <c r="S18" s="20"/>
-      <c r="T18" s="20">
+      <c r="R18" s="22"/>
+      <c r="S18" s="22"/>
+      <c r="T18" s="22">
         <v>19</v>
       </c>
-      <c r="U18" s="20"/>
-      <c r="V18" s="20"/>
-      <c r="W18" s="20"/>
-      <c r="X18" s="20"/>
-      <c r="Y18" s="20">
+      <c r="U18" s="22"/>
+      <c r="V18" s="22"/>
+      <c r="W18" s="22"/>
+      <c r="X18" s="22"/>
+      <c r="Y18" s="22">
         <v>17</v>
       </c>
-      <c r="Z18" s="20"/>
-      <c r="AA18" s="20"/>
-      <c r="AB18" s="20"/>
-      <c r="AC18" s="20"/>
-      <c r="AD18" s="20">
-        <v>0</v>
-      </c>
-      <c r="AE18" s="20"/>
-      <c r="AF18" s="20"/>
+      <c r="Z18" s="22"/>
+      <c r="AA18" s="22"/>
+      <c r="AB18" s="22"/>
+      <c r="AC18" s="22"/>
+      <c r="AD18" s="22">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="22"/>
+      <c r="AF18" s="22"/>
     </row>
     <row r="19" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20" t="s">
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="20" t="s">
+      <c r="O19" s="22"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="R19" s="20"/>
-      <c r="S19" s="20"/>
-      <c r="T19" s="20" t="s">
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
+      <c r="T19" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="U19" s="20"/>
-      <c r="V19" s="20"/>
-      <c r="W19" s="20"/>
-      <c r="X19" s="20"/>
-      <c r="Y19" s="20" t="s">
+      <c r="U19" s="22"/>
+      <c r="V19" s="22"/>
+      <c r="W19" s="22"/>
+      <c r="X19" s="22"/>
+      <c r="Y19" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="Z19" s="20"/>
-      <c r="AA19" s="20"/>
-      <c r="AB19" s="20"/>
-      <c r="AC19" s="20"/>
-      <c r="AD19" s="20" t="s">
+      <c r="Z19" s="22"/>
+      <c r="AA19" s="22"/>
+      <c r="AB19" s="22"/>
+      <c r="AC19" s="22"/>
+      <c r="AD19" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="AE19" s="20"/>
-      <c r="AF19" s="20"/>
+      <c r="AE19" s="22"/>
+      <c r="AF19" s="22"/>
     </row>
     <row r="20" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A20" s="20">
+      <c r="A20" s="22">
         <f>A18</f>
         <v>5</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="21">
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="23">
         <f>'Data package'!$B$31*I18+'Data package'!$B$28</f>
         <v>3.3870967741935485</v>
       </c>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="22">
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="20">
         <f ca="1">LOOKUP(N18,'Data package'!$D$21:$D$24,'Data package'!$E$22:$E$35)</f>
         <v>0</v>
       </c>
-      <c r="O20" s="22"/>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="23">
+      <c r="O20" s="20"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="24">
         <f>100/(2^3-1)*Q18</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R20" s="23"/>
-      <c r="S20" s="23"/>
-      <c r="T20" s="23">
+      <c r="R20" s="24"/>
+      <c r="S20" s="24"/>
+      <c r="T20" s="24">
         <f>'Data package'!$B$40*T18+'Data package'!$B$37</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U20" s="22"/>
-      <c r="V20" s="22"/>
-      <c r="W20" s="22"/>
-      <c r="X20" s="22"/>
-      <c r="Y20" s="22">
+      <c r="U20" s="20"/>
+      <c r="V20" s="20"/>
+      <c r="W20" s="20"/>
+      <c r="X20" s="20"/>
+      <c r="Y20" s="20">
         <f>Y18</f>
         <v>17</v>
       </c>
-      <c r="Z20" s="22"/>
-      <c r="AA20" s="22"/>
-      <c r="AB20" s="22"/>
-      <c r="AC20" s="22"/>
-      <c r="AD20" s="22">
+      <c r="Z20" s="20"/>
+      <c r="AA20" s="20"/>
+      <c r="AB20" s="20"/>
+      <c r="AC20" s="20"/>
+      <c r="AD20" s="20">
         <f>LOOKUP(AD18,'Data package'!$A$84:$A$88,'Data package'!$B$84:$B$88)</f>
         <v>1</v>
       </c>
-      <c r="AE20" s="22"/>
-      <c r="AF20" s="22"/>
+      <c r="AE20" s="20"/>
+      <c r="AF20" s="20"/>
     </row>
     <row r="23" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A23" s="25" t="s">
@@ -4239,126 +5791,126 @@
       <c r="AF23" s="25"/>
     </row>
     <row r="24" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24" t="s">
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="24"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="24"/>
-      <c r="Q24" s="24" t="s">
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="26"/>
+      <c r="Q24" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="R24" s="24"/>
-      <c r="S24" s="24"/>
-      <c r="T24" s="24"/>
-      <c r="U24" s="24"/>
-      <c r="V24" s="24"/>
-      <c r="W24" s="24"/>
-      <c r="X24" s="24"/>
-      <c r="Y24" s="24" t="s">
+      <c r="R24" s="26"/>
+      <c r="S24" s="26"/>
+      <c r="T24" s="26"/>
+      <c r="U24" s="26"/>
+      <c r="V24" s="26"/>
+      <c r="W24" s="26"/>
+      <c r="X24" s="26"/>
+      <c r="Y24" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="Z24" s="24"/>
-      <c r="AA24" s="24"/>
-      <c r="AB24" s="24"/>
-      <c r="AC24" s="24"/>
-      <c r="AD24" s="24"/>
-      <c r="AE24" s="24"/>
-      <c r="AF24" s="24"/>
-      <c r="AG24" s="35">
+      <c r="Z24" s="26"/>
+      <c r="AA24" s="26"/>
+      <c r="AB24" s="26"/>
+      <c r="AC24" s="26"/>
+      <c r="AD24" s="26"/>
+      <c r="AE24" s="26"/>
+      <c r="AF24" s="26"/>
+      <c r="AG24" s="21">
         <v>59</v>
       </c>
-      <c r="AH24" s="35"/>
-      <c r="AI24" s="35"/>
-      <c r="AJ24" s="35"/>
-      <c r="AK24" s="35"/>
-      <c r="AL24" s="35"/>
-      <c r="AM24" s="35"/>
-      <c r="AN24" s="35"/>
-      <c r="AO24" s="35">
+      <c r="AH24" s="21"/>
+      <c r="AI24" s="21"/>
+      <c r="AJ24" s="21"/>
+      <c r="AK24" s="21"/>
+      <c r="AL24" s="21"/>
+      <c r="AM24" s="21"/>
+      <c r="AN24" s="21"/>
+      <c r="AO24" s="21">
         <v>96</v>
       </c>
-      <c r="AP24" s="35"/>
-      <c r="AQ24" s="35"/>
-      <c r="AR24" s="35"/>
-      <c r="AS24" s="35"/>
-      <c r="AT24" s="35"/>
-      <c r="AU24" s="35"/>
-      <c r="AV24" s="35"/>
-      <c r="AW24" s="35">
+      <c r="AP24" s="21"/>
+      <c r="AQ24" s="21"/>
+      <c r="AR24" s="21"/>
+      <c r="AS24" s="21"/>
+      <c r="AT24" s="21"/>
+      <c r="AU24" s="21"/>
+      <c r="AV24" s="21"/>
+      <c r="AW24" s="21">
         <v>65</v>
       </c>
-      <c r="AX24" s="35"/>
-      <c r="AY24" s="35"/>
-      <c r="AZ24" s="35"/>
-      <c r="BA24" s="35"/>
-      <c r="BB24" s="35"/>
-      <c r="BC24" s="35"/>
-      <c r="BD24" s="35"/>
-      <c r="BE24" s="35" t="s">
+      <c r="AX24" s="21"/>
+      <c r="AY24" s="21"/>
+      <c r="AZ24" s="21"/>
+      <c r="BA24" s="21"/>
+      <c r="BB24" s="21"/>
+      <c r="BC24" s="21"/>
+      <c r="BD24" s="21"/>
+      <c r="BE24" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="BF24" s="35"/>
-      <c r="BG24" s="35"/>
-      <c r="BH24" s="35"/>
-      <c r="BI24" s="35"/>
-      <c r="BJ24" s="35"/>
-      <c r="BK24" s="35"/>
-      <c r="BL24" s="35"/>
-      <c r="BM24" s="35" t="s">
+      <c r="BF24" s="21"/>
+      <c r="BG24" s="21"/>
+      <c r="BH24" s="21"/>
+      <c r="BI24" s="21"/>
+      <c r="BJ24" s="21"/>
+      <c r="BK24" s="21"/>
+      <c r="BL24" s="21"/>
+      <c r="BM24" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="BN24" s="35"/>
-      <c r="BO24" s="35"/>
-      <c r="BP24" s="35"/>
-      <c r="BQ24" s="35"/>
-      <c r="BR24" s="35"/>
-      <c r="BS24" s="35"/>
-      <c r="BT24" s="35"/>
-      <c r="BU24" s="35">
+      <c r="BN24" s="21"/>
+      <c r="BO24" s="21"/>
+      <c r="BP24" s="21"/>
+      <c r="BQ24" s="21"/>
+      <c r="BR24" s="21"/>
+      <c r="BS24" s="21"/>
+      <c r="BT24" s="21"/>
+      <c r="BU24" s="21">
         <v>69</v>
       </c>
-      <c r="BV24" s="35"/>
-      <c r="BW24" s="35"/>
-      <c r="BX24" s="35"/>
-      <c r="BY24" s="35"/>
-      <c r="BZ24" s="35"/>
-      <c r="CA24" s="35"/>
-      <c r="CB24" s="35"/>
-      <c r="CC24" s="35" t="s">
+      <c r="BV24" s="21"/>
+      <c r="BW24" s="21"/>
+      <c r="BX24" s="21"/>
+      <c r="BY24" s="21"/>
+      <c r="BZ24" s="21"/>
+      <c r="CA24" s="21"/>
+      <c r="CB24" s="21"/>
+      <c r="CC24" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="CD24" s="35"/>
-      <c r="CE24" s="35"/>
-      <c r="CF24" s="35"/>
-      <c r="CG24" s="35"/>
-      <c r="CH24" s="35"/>
-      <c r="CI24" s="35"/>
-      <c r="CJ24" s="35"/>
-      <c r="CK24" s="35" t="s">
+      <c r="CD24" s="21"/>
+      <c r="CE24" s="21"/>
+      <c r="CF24" s="21"/>
+      <c r="CG24" s="21"/>
+      <c r="CH24" s="21"/>
+      <c r="CI24" s="21"/>
+      <c r="CJ24" s="21"/>
+      <c r="CK24" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="CL24" s="35"/>
-      <c r="CM24" s="35"/>
-      <c r="CN24" s="35"/>
-      <c r="CO24" s="35"/>
-      <c r="CP24" s="35"/>
-      <c r="CQ24" s="35"/>
-      <c r="CR24" s="35"/>
+      <c r="CL24" s="21"/>
+      <c r="CM24" s="21"/>
+      <c r="CN24" s="21"/>
+      <c r="CO24" s="21"/>
+      <c r="CP24" s="21"/>
+      <c r="CQ24" s="21"/>
+      <c r="CR24" s="21"/>
     </row>
     <row r="25" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
@@ -4651,180 +6203,180 @@
       </c>
     </row>
     <row r="26" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20" t="s">
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20" t="s">
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="O26" s="20"/>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="20" t="s">
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="R26" s="20"/>
-      <c r="S26" s="20"/>
-      <c r="T26" s="20" t="s">
+      <c r="R26" s="22"/>
+      <c r="S26" s="22"/>
+      <c r="T26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="U26" s="20"/>
-      <c r="V26" s="20"/>
-      <c r="W26" s="20"/>
-      <c r="X26" s="20"/>
-      <c r="Y26" s="20" t="s">
+      <c r="U26" s="22"/>
+      <c r="V26" s="22"/>
+      <c r="W26" s="22"/>
+      <c r="X26" s="22"/>
+      <c r="Y26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="Z26" s="20"/>
-      <c r="AA26" s="20"/>
-      <c r="AB26" s="20"/>
-      <c r="AC26" s="20"/>
-      <c r="AD26" s="20" t="s">
+      <c r="Z26" s="22"/>
+      <c r="AA26" s="22"/>
+      <c r="AB26" s="22"/>
+      <c r="AC26" s="22"/>
+      <c r="AD26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="AE26" s="20"/>
-      <c r="AF26" s="20"/>
-      <c r="AG26" s="22" t="s">
+      <c r="AE26" s="22"/>
+      <c r="AF26" s="22"/>
+      <c r="AG26" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AH26" s="22"/>
-      <c r="AI26" s="22"/>
-      <c r="AJ26" s="22"/>
-      <c r="AK26" s="22"/>
-      <c r="AL26" s="22"/>
-      <c r="AM26" s="22"/>
-      <c r="AN26" s="22"/>
-      <c r="AO26" s="22" t="s">
+      <c r="AH26" s="20"/>
+      <c r="AI26" s="20"/>
+      <c r="AJ26" s="20"/>
+      <c r="AK26" s="20"/>
+      <c r="AL26" s="20"/>
+      <c r="AM26" s="20"/>
+      <c r="AN26" s="20"/>
+      <c r="AO26" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AP26" s="22"/>
-      <c r="AQ26" s="22"/>
-      <c r="AR26" s="22"/>
-      <c r="AS26" s="22"/>
-      <c r="AT26" s="22"/>
-      <c r="AU26" s="22"/>
-      <c r="AV26" s="22"/>
-      <c r="AW26" s="22" t="s">
+      <c r="AP26" s="20"/>
+      <c r="AQ26" s="20"/>
+      <c r="AR26" s="20"/>
+      <c r="AS26" s="20"/>
+      <c r="AT26" s="20"/>
+      <c r="AU26" s="20"/>
+      <c r="AV26" s="20"/>
+      <c r="AW26" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AX26" s="22"/>
-      <c r="AY26" s="22"/>
-      <c r="AZ26" s="22"/>
-      <c r="BA26" s="22"/>
-      <c r="BB26" s="22"/>
-      <c r="BC26" s="22"/>
-      <c r="BD26" s="22"/>
-      <c r="BE26" s="22" t="s">
+      <c r="AX26" s="20"/>
+      <c r="AY26" s="20"/>
+      <c r="AZ26" s="20"/>
+      <c r="BA26" s="20"/>
+      <c r="BB26" s="20"/>
+      <c r="BC26" s="20"/>
+      <c r="BD26" s="20"/>
+      <c r="BE26" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="BF26" s="22"/>
-      <c r="BG26" s="22"/>
-      <c r="BH26" s="22"/>
-      <c r="BI26" s="22"/>
-      <c r="BJ26" s="22"/>
-      <c r="BK26" s="22"/>
-      <c r="BL26" s="22"/>
-      <c r="BM26" s="22" t="s">
+      <c r="BF26" s="20"/>
+      <c r="BG26" s="20"/>
+      <c r="BH26" s="20"/>
+      <c r="BI26" s="20"/>
+      <c r="BJ26" s="20"/>
+      <c r="BK26" s="20"/>
+      <c r="BL26" s="20"/>
+      <c r="BM26" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="BN26" s="22"/>
-      <c r="BO26" s="22"/>
-      <c r="BP26" s="22"/>
-      <c r="BQ26" s="22"/>
-      <c r="BR26" s="22"/>
-      <c r="BS26" s="22"/>
-      <c r="BT26" s="22"/>
-      <c r="BU26" s="22" t="s">
+      <c r="BN26" s="20"/>
+      <c r="BO26" s="20"/>
+      <c r="BP26" s="20"/>
+      <c r="BQ26" s="20"/>
+      <c r="BR26" s="20"/>
+      <c r="BS26" s="20"/>
+      <c r="BT26" s="20"/>
+      <c r="BU26" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="BV26" s="22"/>
-      <c r="BW26" s="22"/>
-      <c r="BX26" s="22"/>
-      <c r="BY26" s="22"/>
-      <c r="BZ26" s="22"/>
-      <c r="CA26" s="22"/>
-      <c r="CB26" s="22"/>
-      <c r="CC26" s="22" t="s">
+      <c r="BV26" s="20"/>
+      <c r="BW26" s="20"/>
+      <c r="BX26" s="20"/>
+      <c r="BY26" s="20"/>
+      <c r="BZ26" s="20"/>
+      <c r="CA26" s="20"/>
+      <c r="CB26" s="20"/>
+      <c r="CC26" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="CD26" s="22"/>
-      <c r="CE26" s="22"/>
-      <c r="CF26" s="22"/>
-      <c r="CG26" s="22"/>
-      <c r="CH26" s="22"/>
-      <c r="CI26" s="22"/>
-      <c r="CJ26" s="22"/>
-      <c r="CK26" s="22" t="s">
+      <c r="CD26" s="20"/>
+      <c r="CE26" s="20"/>
+      <c r="CF26" s="20"/>
+      <c r="CG26" s="20"/>
+      <c r="CH26" s="20"/>
+      <c r="CI26" s="20"/>
+      <c r="CJ26" s="20"/>
+      <c r="CK26" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="CL26" s="22"/>
-      <c r="CM26" s="22"/>
-      <c r="CN26" s="22"/>
-      <c r="CO26" s="22"/>
-      <c r="CP26" s="22"/>
-      <c r="CQ26" s="22"/>
-      <c r="CR26" s="22"/>
+      <c r="CL26" s="20"/>
+      <c r="CM26" s="20"/>
+      <c r="CN26" s="20"/>
+      <c r="CO26" s="20"/>
+      <c r="CP26" s="20"/>
+      <c r="CQ26" s="20"/>
+      <c r="CR26" s="20"/>
     </row>
     <row r="27" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A27" s="20">
+      <c r="A27" s="22">
         <v>10</v>
       </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20">
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22">
         <v>8</v>
       </c>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20">
-        <v>0</v>
-      </c>
-      <c r="O27" s="20"/>
-      <c r="P27" s="20"/>
-      <c r="Q27" s="20">
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22">
+        <v>0</v>
+      </c>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22">
         <v>3</v>
       </c>
-      <c r="R27" s="20"/>
-      <c r="S27" s="20"/>
-      <c r="T27" s="20">
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="22">
         <v>19</v>
       </c>
-      <c r="U27" s="20"/>
-      <c r="V27" s="20"/>
-      <c r="W27" s="20"/>
-      <c r="X27" s="20"/>
-      <c r="Y27" s="20">
+      <c r="U27" s="22"/>
+      <c r="V27" s="22"/>
+      <c r="W27" s="22"/>
+      <c r="X27" s="22"/>
+      <c r="Y27" s="22">
         <v>21</v>
       </c>
-      <c r="Z27" s="20"/>
-      <c r="AA27" s="20"/>
-      <c r="AB27" s="20"/>
-      <c r="AC27" s="20"/>
-      <c r="AD27" s="20">
-        <v>0</v>
-      </c>
-      <c r="AE27" s="20"/>
-      <c r="AF27" s="20"/>
+      <c r="Z27" s="22"/>
+      <c r="AA27" s="22"/>
+      <c r="AB27" s="22"/>
+      <c r="AC27" s="22"/>
+      <c r="AD27" s="22">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="22"/>
+      <c r="AF27" s="22"/>
       <c r="AG27">
         <f>AN25</f>
         <v>1</v>
@@ -5083,267 +6635,267 @@
       </c>
     </row>
     <row r="28" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20" t="s">
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="20"/>
-      <c r="M28" s="20"/>
-      <c r="N28" s="20" t="s">
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="O28" s="20"/>
-      <c r="P28" s="20"/>
-      <c r="Q28" s="20" t="s">
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="R28" s="20"/>
-      <c r="S28" s="20"/>
-      <c r="T28" s="20" t="s">
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="U28" s="20"/>
-      <c r="V28" s="20"/>
-      <c r="W28" s="20"/>
-      <c r="X28" s="20"/>
-      <c r="Y28" s="20" t="s">
+      <c r="U28" s="22"/>
+      <c r="V28" s="22"/>
+      <c r="W28" s="22"/>
+      <c r="X28" s="22"/>
+      <c r="Y28" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="Z28" s="20"/>
-      <c r="AA28" s="20"/>
-      <c r="AB28" s="20"/>
-      <c r="AC28" s="20"/>
-      <c r="AD28" s="20" t="s">
+      <c r="Z28" s="22"/>
+      <c r="AA28" s="22"/>
+      <c r="AB28" s="22"/>
+      <c r="AC28" s="22"/>
+      <c r="AD28" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="AE28" s="20"/>
-      <c r="AF28" s="20"/>
-      <c r="AG28" s="22" t="s">
+      <c r="AE28" s="22"/>
+      <c r="AF28" s="22"/>
+      <c r="AG28" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="AH28" s="22"/>
-      <c r="AI28" s="22"/>
-      <c r="AJ28" s="22"/>
-      <c r="AK28" s="22"/>
-      <c r="AL28" s="22"/>
-      <c r="AM28" s="22" t="s">
+      <c r="AH28" s="20"/>
+      <c r="AI28" s="20"/>
+      <c r="AJ28" s="20"/>
+      <c r="AK28" s="20"/>
+      <c r="AL28" s="20"/>
+      <c r="AM28" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="AN28" s="22"/>
-      <c r="AO28" s="22"/>
-      <c r="AP28" s="22"/>
-      <c r="AQ28" s="22"/>
-      <c r="AR28" s="22"/>
-      <c r="AS28" s="22" t="s">
+      <c r="AN28" s="20"/>
+      <c r="AO28" s="20"/>
+      <c r="AP28" s="20"/>
+      <c r="AQ28" s="20"/>
+      <c r="AR28" s="20"/>
+      <c r="AS28" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="AT28" s="22"/>
-      <c r="AU28" s="22"/>
-      <c r="AV28" s="22"/>
-      <c r="AW28" s="22"/>
-      <c r="AX28" s="22"/>
-      <c r="AY28" s="22" t="s">
+      <c r="AT28" s="20"/>
+      <c r="AU28" s="20"/>
+      <c r="AV28" s="20"/>
+      <c r="AW28" s="20"/>
+      <c r="AX28" s="20"/>
+      <c r="AY28" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="AZ28" s="22"/>
-      <c r="BA28" s="22"/>
-      <c r="BB28" s="22"/>
-      <c r="BC28" s="22"/>
-      <c r="BD28" s="22"/>
-      <c r="BE28" s="22" t="s">
+      <c r="AZ28" s="20"/>
+      <c r="BA28" s="20"/>
+      <c r="BB28" s="20"/>
+      <c r="BC28" s="20"/>
+      <c r="BD28" s="20"/>
+      <c r="BE28" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="BF28" s="22"/>
-      <c r="BG28" s="22"/>
-      <c r="BH28" s="22"/>
-      <c r="BI28" s="22"/>
-      <c r="BJ28" s="22"/>
-      <c r="BK28" s="22" t="s">
+      <c r="BF28" s="20"/>
+      <c r="BG28" s="20"/>
+      <c r="BH28" s="20"/>
+      <c r="BI28" s="20"/>
+      <c r="BJ28" s="20"/>
+      <c r="BK28" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="BL28" s="22"/>
-      <c r="BM28" s="22"/>
-      <c r="BN28" s="22"/>
-      <c r="BO28" s="22"/>
-      <c r="BP28" s="22"/>
-      <c r="BQ28" s="22" t="s">
+      <c r="BL28" s="20"/>
+      <c r="BM28" s="20"/>
+      <c r="BN28" s="20"/>
+      <c r="BO28" s="20"/>
+      <c r="BP28" s="20"/>
+      <c r="BQ28" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="BR28" s="22"/>
-      <c r="BS28" s="22"/>
-      <c r="BT28" s="22"/>
-      <c r="BU28" s="22"/>
-      <c r="BV28" s="22"/>
-      <c r="BW28" s="22" t="s">
+      <c r="BR28" s="20"/>
+      <c r="BS28" s="20"/>
+      <c r="BT28" s="20"/>
+      <c r="BU28" s="20"/>
+      <c r="BV28" s="20"/>
+      <c r="BW28" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="BX28" s="22"/>
-      <c r="BY28" s="22"/>
-      <c r="BZ28" s="22"/>
-      <c r="CA28" s="22"/>
-      <c r="CB28" s="22"/>
-      <c r="CC28" s="22" t="s">
+      <c r="BX28" s="20"/>
+      <c r="BY28" s="20"/>
+      <c r="BZ28" s="20"/>
+      <c r="CA28" s="20"/>
+      <c r="CB28" s="20"/>
+      <c r="CC28" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="CD28" s="22"/>
-      <c r="CE28" s="22"/>
-      <c r="CF28" s="22"/>
-      <c r="CG28" s="22"/>
-      <c r="CH28" s="22"/>
-      <c r="CI28" s="22" t="s">
+      <c r="CD28" s="20"/>
+      <c r="CE28" s="20"/>
+      <c r="CF28" s="20"/>
+      <c r="CG28" s="20"/>
+      <c r="CH28" s="20"/>
+      <c r="CI28" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="CJ28" s="22"/>
-      <c r="CK28" s="22"/>
-      <c r="CL28" s="22"/>
-      <c r="CM28" s="22"/>
-      <c r="CN28" s="22"/>
+      <c r="CJ28" s="20"/>
+      <c r="CK28" s="20"/>
+      <c r="CL28" s="20"/>
+      <c r="CM28" s="20"/>
+      <c r="CN28" s="20"/>
     </row>
     <row r="29" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A29" s="20">
+      <c r="A29" s="22">
         <f>A27</f>
         <v>10</v>
       </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="21">
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="23">
         <f>'Data package'!$B$31*I27+'Data package'!$B$28</f>
         <v>3.3870967741935485</v>
       </c>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="21"/>
-      <c r="M29" s="21"/>
-      <c r="N29" s="22">
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="20">
         <f ca="1">LOOKUP(N27,'Data package'!$D$21:$D$24,'Data package'!$E$22:$E$35)</f>
         <v>0</v>
       </c>
-      <c r="O29" s="22"/>
-      <c r="P29" s="22"/>
-      <c r="Q29" s="23">
+      <c r="O29" s="20"/>
+      <c r="P29" s="20"/>
+      <c r="Q29" s="24">
         <f>100/(2^3-1)*Q27</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R29" s="23"/>
-      <c r="S29" s="23"/>
-      <c r="T29" s="23">
+      <c r="R29" s="24"/>
+      <c r="S29" s="24"/>
+      <c r="T29" s="24">
         <f>'Data package'!$B$40*T27+'Data package'!$B$37</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U29" s="22"/>
-      <c r="V29" s="22"/>
-      <c r="W29" s="22"/>
-      <c r="X29" s="22"/>
-      <c r="Y29" s="22">
+      <c r="U29" s="20"/>
+      <c r="V29" s="20"/>
+      <c r="W29" s="20"/>
+      <c r="X29" s="20"/>
+      <c r="Y29" s="20">
         <f>Y27</f>
         <v>21</v>
       </c>
-      <c r="Z29" s="22"/>
-      <c r="AA29" s="22"/>
-      <c r="AB29" s="22"/>
-      <c r="AC29" s="22"/>
-      <c r="AD29" s="22">
+      <c r="Z29" s="20"/>
+      <c r="AA29" s="20"/>
+      <c r="AB29" s="20"/>
+      <c r="AC29" s="20"/>
+      <c r="AD29" s="20">
         <f>LOOKUP(AD27,'Data package'!$A$84:$A$88,'Data package'!$B$84:$B$88)</f>
         <v>1</v>
       </c>
-      <c r="AE29" s="22"/>
-      <c r="AF29" s="22"/>
-      <c r="AG29" s="22" t="s">
+      <c r="AE29" s="20"/>
+      <c r="AF29" s="20"/>
+      <c r="AG29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AH29" s="22"/>
-      <c r="AI29" s="22"/>
-      <c r="AJ29" s="22"/>
-      <c r="AK29" s="22"/>
-      <c r="AL29" s="22"/>
-      <c r="AM29" s="22" t="s">
+      <c r="AH29" s="20"/>
+      <c r="AI29" s="20"/>
+      <c r="AJ29" s="20"/>
+      <c r="AK29" s="20"/>
+      <c r="AL29" s="20"/>
+      <c r="AM29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AN29" s="22"/>
-      <c r="AO29" s="22"/>
-      <c r="AP29" s="22"/>
-      <c r="AQ29" s="22"/>
-      <c r="AR29" s="22"/>
-      <c r="AS29" s="22" t="s">
+      <c r="AN29" s="20"/>
+      <c r="AO29" s="20"/>
+      <c r="AP29" s="20"/>
+      <c r="AQ29" s="20"/>
+      <c r="AR29" s="20"/>
+      <c r="AS29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AT29" s="22"/>
-      <c r="AU29" s="22"/>
-      <c r="AV29" s="22"/>
-      <c r="AW29" s="22"/>
-      <c r="AX29" s="22"/>
-      <c r="AY29" s="22" t="s">
+      <c r="AT29" s="20"/>
+      <c r="AU29" s="20"/>
+      <c r="AV29" s="20"/>
+      <c r="AW29" s="20"/>
+      <c r="AX29" s="20"/>
+      <c r="AY29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AZ29" s="22"/>
-      <c r="BA29" s="22"/>
-      <c r="BB29" s="22"/>
-      <c r="BC29" s="22"/>
-      <c r="BD29" s="22"/>
-      <c r="BE29" s="22" t="s">
+      <c r="AZ29" s="20"/>
+      <c r="BA29" s="20"/>
+      <c r="BB29" s="20"/>
+      <c r="BC29" s="20"/>
+      <c r="BD29" s="20"/>
+      <c r="BE29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="BF29" s="22"/>
-      <c r="BG29" s="22"/>
-      <c r="BH29" s="22"/>
-      <c r="BI29" s="22"/>
-      <c r="BJ29" s="22"/>
-      <c r="BK29" s="22" t="s">
+      <c r="BF29" s="20"/>
+      <c r="BG29" s="20"/>
+      <c r="BH29" s="20"/>
+      <c r="BI29" s="20"/>
+      <c r="BJ29" s="20"/>
+      <c r="BK29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="BL29" s="22"/>
-      <c r="BM29" s="22"/>
-      <c r="BN29" s="22"/>
-      <c r="BO29" s="22"/>
-      <c r="BP29" s="22"/>
-      <c r="BQ29" s="22" t="s">
+      <c r="BL29" s="20"/>
+      <c r="BM29" s="20"/>
+      <c r="BN29" s="20"/>
+      <c r="BO29" s="20"/>
+      <c r="BP29" s="20"/>
+      <c r="BQ29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="BR29" s="22"/>
-      <c r="BS29" s="22"/>
-      <c r="BT29" s="22"/>
-      <c r="BU29" s="22"/>
-      <c r="BV29" s="22"/>
-      <c r="BW29" s="22" t="s">
+      <c r="BR29" s="20"/>
+      <c r="BS29" s="20"/>
+      <c r="BT29" s="20"/>
+      <c r="BU29" s="20"/>
+      <c r="BV29" s="20"/>
+      <c r="BW29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="BX29" s="22"/>
-      <c r="BY29" s="22"/>
-      <c r="BZ29" s="22"/>
-      <c r="CA29" s="22"/>
-      <c r="CB29" s="22"/>
-      <c r="CC29" s="22" t="s">
+      <c r="BX29" s="20"/>
+      <c r="BY29" s="20"/>
+      <c r="BZ29" s="20"/>
+      <c r="CA29" s="20"/>
+      <c r="CB29" s="20"/>
+      <c r="CC29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="CD29" s="22"/>
-      <c r="CE29" s="22"/>
-      <c r="CF29" s="22"/>
-      <c r="CG29" s="22"/>
-      <c r="CH29" s="22"/>
-      <c r="CI29" s="22" t="s">
+      <c r="CD29" s="20"/>
+      <c r="CE29" s="20"/>
+      <c r="CF29" s="20"/>
+      <c r="CG29" s="20"/>
+      <c r="CH29" s="20"/>
+      <c r="CI29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="CJ29" s="22"/>
-      <c r="CK29" s="22"/>
-      <c r="CL29" s="22"/>
-      <c r="CM29" s="22"/>
-      <c r="CN29" s="22"/>
+      <c r="CJ29" s="20"/>
+      <c r="CK29" s="20"/>
+      <c r="CL29" s="20"/>
+      <c r="CM29" s="20"/>
+      <c r="CN29" s="20"/>
     </row>
     <row r="30" spans="1:96" x14ac:dyDescent="0.3">
       <c r="AG30">
@@ -5588,255 +7140,229 @@
       </c>
     </row>
     <row r="31" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="AG31" s="22" t="s">
+      <c r="AG31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="AH31" s="22"/>
-      <c r="AI31" s="22"/>
-      <c r="AJ31" s="22"/>
-      <c r="AK31" s="22"/>
-      <c r="AL31" s="22"/>
-      <c r="AM31" s="22" t="s">
+      <c r="AH31" s="20"/>
+      <c r="AI31" s="20"/>
+      <c r="AJ31" s="20"/>
+      <c r="AK31" s="20"/>
+      <c r="AL31" s="20"/>
+      <c r="AM31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="AN31" s="22"/>
-      <c r="AO31" s="22"/>
-      <c r="AP31" s="22"/>
-      <c r="AQ31" s="22"/>
-      <c r="AR31" s="22"/>
-      <c r="AS31" s="22" t="s">
+      <c r="AN31" s="20"/>
+      <c r="AO31" s="20"/>
+      <c r="AP31" s="20"/>
+      <c r="AQ31" s="20"/>
+      <c r="AR31" s="20"/>
+      <c r="AS31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="AT31" s="22"/>
-      <c r="AU31" s="22"/>
-      <c r="AV31" s="22"/>
-      <c r="AW31" s="22"/>
-      <c r="AX31" s="22"/>
-      <c r="AY31" s="22" t="s">
+      <c r="AT31" s="20"/>
+      <c r="AU31" s="20"/>
+      <c r="AV31" s="20"/>
+      <c r="AW31" s="20"/>
+      <c r="AX31" s="20"/>
+      <c r="AY31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="AZ31" s="22"/>
-      <c r="BA31" s="22"/>
-      <c r="BB31" s="22"/>
-      <c r="BC31" s="22"/>
-      <c r="BD31" s="22"/>
-      <c r="BE31" s="22" t="s">
+      <c r="AZ31" s="20"/>
+      <c r="BA31" s="20"/>
+      <c r="BB31" s="20"/>
+      <c r="BC31" s="20"/>
+      <c r="BD31" s="20"/>
+      <c r="BE31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="BF31" s="22"/>
-      <c r="BG31" s="22"/>
-      <c r="BH31" s="22"/>
-      <c r="BI31" s="22"/>
-      <c r="BJ31" s="22"/>
-      <c r="BK31" s="22" t="s">
+      <c r="BF31" s="20"/>
+      <c r="BG31" s="20"/>
+      <c r="BH31" s="20"/>
+      <c r="BI31" s="20"/>
+      <c r="BJ31" s="20"/>
+      <c r="BK31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="BL31" s="22"/>
-      <c r="BM31" s="22"/>
-      <c r="BN31" s="22"/>
-      <c r="BO31" s="22"/>
-      <c r="BP31" s="22"/>
-      <c r="BQ31" s="22" t="s">
+      <c r="BL31" s="20"/>
+      <c r="BM31" s="20"/>
+      <c r="BN31" s="20"/>
+      <c r="BO31" s="20"/>
+      <c r="BP31" s="20"/>
+      <c r="BQ31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="BR31" s="22"/>
-      <c r="BS31" s="22"/>
-      <c r="BT31" s="22"/>
-      <c r="BU31" s="22"/>
-      <c r="BV31" s="22"/>
-      <c r="BW31" s="22" t="s">
+      <c r="BR31" s="20"/>
+      <c r="BS31" s="20"/>
+      <c r="BT31" s="20"/>
+      <c r="BU31" s="20"/>
+      <c r="BV31" s="20"/>
+      <c r="BW31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="BX31" s="22"/>
-      <c r="BY31" s="22"/>
-      <c r="BZ31" s="22"/>
-      <c r="CA31" s="22"/>
-      <c r="CB31" s="22"/>
-      <c r="CC31" s="22" t="s">
+      <c r="BX31" s="20"/>
+      <c r="BY31" s="20"/>
+      <c r="BZ31" s="20"/>
+      <c r="CA31" s="20"/>
+      <c r="CB31" s="20"/>
+      <c r="CC31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="CD31" s="22"/>
-      <c r="CE31" s="22"/>
-      <c r="CF31" s="22"/>
-      <c r="CG31" s="22"/>
-      <c r="CH31" s="22"/>
-      <c r="CI31" s="22" t="s">
+      <c r="CD31" s="20"/>
+      <c r="CE31" s="20"/>
+      <c r="CF31" s="20"/>
+      <c r="CG31" s="20"/>
+      <c r="CH31" s="20"/>
+      <c r="CI31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="CJ31" s="22"/>
-      <c r="CK31" s="22"/>
-      <c r="CL31" s="22"/>
-      <c r="CM31" s="22"/>
-      <c r="CN31" s="22"/>
+      <c r="CJ31" s="20"/>
+      <c r="CK31" s="20"/>
+      <c r="CL31" s="20"/>
+      <c r="CM31" s="20"/>
+      <c r="CN31" s="20"/>
     </row>
     <row r="32" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="AG32" s="22">
+      <c r="AG32" s="20">
         <v>25</v>
       </c>
-      <c r="AH32" s="22"/>
-      <c r="AI32" s="22"/>
-      <c r="AJ32" s="22"/>
-      <c r="AK32" s="22"/>
-      <c r="AL32" s="22"/>
-      <c r="AM32" s="22">
+      <c r="AH32" s="20"/>
+      <c r="AI32" s="20"/>
+      <c r="AJ32" s="20"/>
+      <c r="AK32" s="20"/>
+      <c r="AL32" s="20"/>
+      <c r="AM32" s="20">
         <v>25</v>
       </c>
-      <c r="AN32" s="22"/>
-      <c r="AO32" s="22"/>
-      <c r="AP32" s="22"/>
-      <c r="AQ32" s="22"/>
-      <c r="AR32" s="22"/>
-      <c r="AS32" s="22">
+      <c r="AN32" s="20"/>
+      <c r="AO32" s="20"/>
+      <c r="AP32" s="20"/>
+      <c r="AQ32" s="20"/>
+      <c r="AR32" s="20"/>
+      <c r="AS32" s="20">
         <v>25</v>
       </c>
-      <c r="AT32" s="22"/>
-      <c r="AU32" s="22"/>
-      <c r="AV32" s="22"/>
-      <c r="AW32" s="22"/>
-      <c r="AX32" s="22"/>
-      <c r="AY32" s="22">
+      <c r="AT32" s="20"/>
+      <c r="AU32" s="20"/>
+      <c r="AV32" s="20"/>
+      <c r="AW32" s="20"/>
+      <c r="AX32" s="20"/>
+      <c r="AY32" s="20">
         <v>25</v>
       </c>
-      <c r="AZ32" s="22"/>
-      <c r="BA32" s="22"/>
-      <c r="BB32" s="22"/>
-      <c r="BC32" s="22"/>
-      <c r="BD32" s="22"/>
-      <c r="BE32" s="22">
+      <c r="AZ32" s="20"/>
+      <c r="BA32" s="20"/>
+      <c r="BB32" s="20"/>
+      <c r="BC32" s="20"/>
+      <c r="BD32" s="20"/>
+      <c r="BE32" s="20">
         <v>26</v>
       </c>
-      <c r="BF32" s="22"/>
-      <c r="BG32" s="22"/>
-      <c r="BH32" s="22"/>
-      <c r="BI32" s="22"/>
-      <c r="BJ32" s="22"/>
-      <c r="BK32" s="22">
+      <c r="BF32" s="20"/>
+      <c r="BG32" s="20"/>
+      <c r="BH32" s="20"/>
+      <c r="BI32" s="20"/>
+      <c r="BJ32" s="20"/>
+      <c r="BK32" s="20">
         <v>26</v>
       </c>
-      <c r="BL32" s="22"/>
-      <c r="BM32" s="22"/>
-      <c r="BN32" s="22"/>
-      <c r="BO32" s="22"/>
-      <c r="BP32" s="22"/>
-      <c r="BQ32" s="22">
+      <c r="BL32" s="20"/>
+      <c r="BM32" s="20"/>
+      <c r="BN32" s="20"/>
+      <c r="BO32" s="20"/>
+      <c r="BP32" s="20"/>
+      <c r="BQ32" s="20">
         <v>26</v>
       </c>
-      <c r="BR32" s="22"/>
-      <c r="BS32" s="22"/>
-      <c r="BT32" s="22"/>
-      <c r="BU32" s="22"/>
-      <c r="BV32" s="22"/>
-      <c r="BW32" s="22">
+      <c r="BR32" s="20"/>
+      <c r="BS32" s="20"/>
+      <c r="BT32" s="20"/>
+      <c r="BU32" s="20"/>
+      <c r="BV32" s="20"/>
+      <c r="BW32" s="20">
         <v>26</v>
       </c>
-      <c r="BX32" s="22"/>
-      <c r="BY32" s="22"/>
-      <c r="BZ32" s="22"/>
-      <c r="CA32" s="22"/>
-      <c r="CB32" s="22"/>
-      <c r="CC32" s="22">
+      <c r="BX32" s="20"/>
+      <c r="BY32" s="20"/>
+      <c r="BZ32" s="20"/>
+      <c r="CA32" s="20"/>
+      <c r="CB32" s="20"/>
+      <c r="CC32" s="20">
         <v>26</v>
       </c>
-      <c r="CD32" s="22"/>
-      <c r="CE32" s="22"/>
-      <c r="CF32" s="22"/>
-      <c r="CG32" s="22"/>
-      <c r="CH32" s="22"/>
-      <c r="CI32" s="22">
+      <c r="CD32" s="20"/>
+      <c r="CE32" s="20"/>
+      <c r="CF32" s="20"/>
+      <c r="CG32" s="20"/>
+      <c r="CH32" s="20"/>
+      <c r="CI32" s="20">
         <v>26</v>
       </c>
-      <c r="CJ32" s="22"/>
-      <c r="CK32" s="22"/>
-      <c r="CL32" s="22"/>
-      <c r="CM32" s="22"/>
-      <c r="CN32" s="22"/>
+      <c r="CJ32" s="20"/>
+      <c r="CK32" s="20"/>
+      <c r="CL32" s="20"/>
+      <c r="CM32" s="20"/>
+      <c r="CN32" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="166">
-    <mergeCell ref="BK32:BP32"/>
-    <mergeCell ref="BQ32:BV32"/>
-    <mergeCell ref="BW32:CB32"/>
-    <mergeCell ref="CC32:CH32"/>
-    <mergeCell ref="CI32:CN32"/>
-    <mergeCell ref="AG32:AL32"/>
-    <mergeCell ref="AM32:AR32"/>
-    <mergeCell ref="AS32:AX32"/>
-    <mergeCell ref="AY32:BD32"/>
-    <mergeCell ref="BE32:BJ32"/>
-    <mergeCell ref="BK31:BP31"/>
-    <mergeCell ref="BQ31:BV31"/>
-    <mergeCell ref="BW31:CB31"/>
-    <mergeCell ref="CC31:CH31"/>
-    <mergeCell ref="CI31:CN31"/>
-    <mergeCell ref="AG31:AL31"/>
-    <mergeCell ref="AM31:AR31"/>
-    <mergeCell ref="AS31:AX31"/>
-    <mergeCell ref="AY31:BD31"/>
-    <mergeCell ref="BE31:BJ31"/>
-    <mergeCell ref="BK29:BP29"/>
-    <mergeCell ref="BQ29:BV29"/>
-    <mergeCell ref="BW29:CB29"/>
-    <mergeCell ref="CC29:CH29"/>
-    <mergeCell ref="CI29:CN29"/>
-    <mergeCell ref="AG29:AL29"/>
-    <mergeCell ref="AM29:AR29"/>
-    <mergeCell ref="AS29:AX29"/>
-    <mergeCell ref="AY29:BD29"/>
-    <mergeCell ref="BE29:BJ29"/>
-    <mergeCell ref="BK28:BP28"/>
-    <mergeCell ref="BQ28:BV28"/>
-    <mergeCell ref="BW28:CB28"/>
-    <mergeCell ref="CC28:CH28"/>
-    <mergeCell ref="CI28:CN28"/>
-    <mergeCell ref="AG28:AL28"/>
-    <mergeCell ref="AM28:AR28"/>
-    <mergeCell ref="AS28:AX28"/>
-    <mergeCell ref="AY28:BD28"/>
-    <mergeCell ref="BE28:BJ28"/>
-    <mergeCell ref="BU24:CB24"/>
-    <mergeCell ref="CC24:CJ24"/>
-    <mergeCell ref="CK24:CR24"/>
-    <mergeCell ref="AG26:AN26"/>
-    <mergeCell ref="AO26:AV26"/>
-    <mergeCell ref="AW26:BD26"/>
-    <mergeCell ref="BE26:BL26"/>
-    <mergeCell ref="BM26:BT26"/>
-    <mergeCell ref="BU26:CB26"/>
-    <mergeCell ref="CC26:CJ26"/>
-    <mergeCell ref="CK26:CR26"/>
-    <mergeCell ref="AG24:AN24"/>
-    <mergeCell ref="AO24:AV24"/>
-    <mergeCell ref="AW24:BD24"/>
-    <mergeCell ref="BE24:BL24"/>
-    <mergeCell ref="BM24:BT24"/>
-    <mergeCell ref="Y28:AC28"/>
-    <mergeCell ref="AD28:AF28"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="I29:M29"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="Q29:S29"/>
-    <mergeCell ref="T29:X29"/>
-    <mergeCell ref="Y29:AC29"/>
-    <mergeCell ref="AD29:AF29"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="I28:M28"/>
-    <mergeCell ref="N28:P28"/>
-    <mergeCell ref="Q28:S28"/>
-    <mergeCell ref="T28:X28"/>
-    <mergeCell ref="Y26:AC26"/>
-    <mergeCell ref="AD26:AF26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="I27:M27"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="Q27:S27"/>
-    <mergeCell ref="T27:X27"/>
-    <mergeCell ref="Y27:AC27"/>
-    <mergeCell ref="AD27:AF27"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="I26:M26"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="Q26:S26"/>
-    <mergeCell ref="T26:X26"/>
+    <mergeCell ref="Y19:AC19"/>
+    <mergeCell ref="AD19:AF19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="I20:M20"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="T20:X20"/>
+    <mergeCell ref="Y20:AC20"/>
+    <mergeCell ref="AD20:AF20"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="I19:M19"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="T19:X19"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="I15:P15"/>
+    <mergeCell ref="Q15:X15"/>
+    <mergeCell ref="Y15:AF15"/>
+    <mergeCell ref="A14:AF14"/>
+    <mergeCell ref="Y17:AC17"/>
+    <mergeCell ref="AD17:AF17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="I18:M18"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="T18:X18"/>
+    <mergeCell ref="Y18:AC18"/>
+    <mergeCell ref="AD18:AF18"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="I17:M17"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="T17:X17"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="I10:M10"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="AD10:AF10"/>
+    <mergeCell ref="Y10:AC10"/>
+    <mergeCell ref="T10:X10"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="AD11:AF11"/>
+    <mergeCell ref="Y11:AC11"/>
+    <mergeCell ref="T11:X11"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="Q6:X6"/>
+    <mergeCell ref="Y6:AF6"/>
+    <mergeCell ref="AD9:AF9"/>
+    <mergeCell ref="AD8:AF8"/>
+    <mergeCell ref="Y9:AC9"/>
+    <mergeCell ref="Y8:AC8"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="T8:X8"/>
+    <mergeCell ref="T9:X9"/>
     <mergeCell ref="A23:AF23"/>
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="I24:P24"/>
@@ -5861,64 +7387,90 @@
     <mergeCell ref="I8:M8"/>
     <mergeCell ref="N8:P8"/>
     <mergeCell ref="I9:M9"/>
-    <mergeCell ref="Q6:X6"/>
-    <mergeCell ref="Y6:AF6"/>
-    <mergeCell ref="AD9:AF9"/>
-    <mergeCell ref="AD8:AF8"/>
-    <mergeCell ref="Y9:AC9"/>
-    <mergeCell ref="Y8:AC8"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="T8:X8"/>
-    <mergeCell ref="T9:X9"/>
-    <mergeCell ref="I11:M11"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="I10:M10"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="AD10:AF10"/>
-    <mergeCell ref="Y10:AC10"/>
-    <mergeCell ref="T10:X10"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="AD11:AF11"/>
-    <mergeCell ref="Y11:AC11"/>
-    <mergeCell ref="T11:X11"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="I15:P15"/>
-    <mergeCell ref="Q15:X15"/>
-    <mergeCell ref="Y15:AF15"/>
-    <mergeCell ref="A14:AF14"/>
-    <mergeCell ref="Y17:AC17"/>
-    <mergeCell ref="AD17:AF17"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="I18:M18"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="T18:X18"/>
-    <mergeCell ref="Y18:AC18"/>
-    <mergeCell ref="AD18:AF18"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="I17:M17"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="T17:X17"/>
-    <mergeCell ref="Y19:AC19"/>
-    <mergeCell ref="AD19:AF19"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="I20:M20"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="T20:X20"/>
-    <mergeCell ref="Y20:AC20"/>
-    <mergeCell ref="AD20:AF20"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="I19:M19"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="T19:X19"/>
+    <mergeCell ref="Y26:AC26"/>
+    <mergeCell ref="AD26:AF26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="I27:M27"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="Q27:S27"/>
+    <mergeCell ref="T27:X27"/>
+    <mergeCell ref="Y27:AC27"/>
+    <mergeCell ref="AD27:AF27"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="I26:M26"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="Q26:S26"/>
+    <mergeCell ref="T26:X26"/>
+    <mergeCell ref="Y28:AC28"/>
+    <mergeCell ref="AD28:AF28"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="I29:M29"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="Q29:S29"/>
+    <mergeCell ref="T29:X29"/>
+    <mergeCell ref="Y29:AC29"/>
+    <mergeCell ref="AD29:AF29"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="I28:M28"/>
+    <mergeCell ref="N28:P28"/>
+    <mergeCell ref="Q28:S28"/>
+    <mergeCell ref="T28:X28"/>
+    <mergeCell ref="BU24:CB24"/>
+    <mergeCell ref="CC24:CJ24"/>
+    <mergeCell ref="CK24:CR24"/>
+    <mergeCell ref="AG26:AN26"/>
+    <mergeCell ref="AO26:AV26"/>
+    <mergeCell ref="AW26:BD26"/>
+    <mergeCell ref="BE26:BL26"/>
+    <mergeCell ref="BM26:BT26"/>
+    <mergeCell ref="BU26:CB26"/>
+    <mergeCell ref="CC26:CJ26"/>
+    <mergeCell ref="CK26:CR26"/>
+    <mergeCell ref="AG24:AN24"/>
+    <mergeCell ref="AO24:AV24"/>
+    <mergeCell ref="AW24:BD24"/>
+    <mergeCell ref="BE24:BL24"/>
+    <mergeCell ref="BM24:BT24"/>
+    <mergeCell ref="BK28:BP28"/>
+    <mergeCell ref="BQ28:BV28"/>
+    <mergeCell ref="BW28:CB28"/>
+    <mergeCell ref="CC28:CH28"/>
+    <mergeCell ref="CI28:CN28"/>
+    <mergeCell ref="AG28:AL28"/>
+    <mergeCell ref="AM28:AR28"/>
+    <mergeCell ref="AS28:AX28"/>
+    <mergeCell ref="AY28:BD28"/>
+    <mergeCell ref="BE28:BJ28"/>
+    <mergeCell ref="BK29:BP29"/>
+    <mergeCell ref="BQ29:BV29"/>
+    <mergeCell ref="BW29:CB29"/>
+    <mergeCell ref="CC29:CH29"/>
+    <mergeCell ref="CI29:CN29"/>
+    <mergeCell ref="AG29:AL29"/>
+    <mergeCell ref="AM29:AR29"/>
+    <mergeCell ref="AS29:AX29"/>
+    <mergeCell ref="AY29:BD29"/>
+    <mergeCell ref="BE29:BJ29"/>
+    <mergeCell ref="BK31:BP31"/>
+    <mergeCell ref="BQ31:BV31"/>
+    <mergeCell ref="BW31:CB31"/>
+    <mergeCell ref="CC31:CH31"/>
+    <mergeCell ref="CI31:CN31"/>
+    <mergeCell ref="AG31:AL31"/>
+    <mergeCell ref="AM31:AR31"/>
+    <mergeCell ref="AS31:AX31"/>
+    <mergeCell ref="AY31:BD31"/>
+    <mergeCell ref="BE31:BJ31"/>
+    <mergeCell ref="BK32:BP32"/>
+    <mergeCell ref="BQ32:BV32"/>
+    <mergeCell ref="BW32:CB32"/>
+    <mergeCell ref="CC32:CH32"/>
+    <mergeCell ref="CI32:CN32"/>
+    <mergeCell ref="AG32:AL32"/>
+    <mergeCell ref="AM32:AR32"/>
+    <mergeCell ref="AS32:AX32"/>
+    <mergeCell ref="AY32:BD32"/>
+    <mergeCell ref="BE32:BJ32"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -5947,11 +7499,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
       <c r="E1" s="7">
         <v>0.5</v>
       </c>
@@ -6572,10 +8124,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C77FA5AC-5DA0-4811-9662-3132B719B7F9}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6680,6 +8232,425 @@
       <c r="B13">
         <v>0</v>
       </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C30" t="s">
+        <v>126</v>
+      </c>
+      <c r="E30" t="s">
+        <v>120</v>
+      </c>
+      <c r="F30">
+        <v>-35946.107099583001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="16">
+        <v>4.2</v>
+      </c>
+      <c r="B31" s="16">
+        <v>100</v>
+      </c>
+      <c r="C31" s="16">
+        <f>$F$35*(A31^5)+$F$34*A31^4+$F$33*A31^3+$F$32*A31^2+$F$31*A31+$F$30</f>
+        <v>100.04675371996564</v>
+      </c>
+      <c r="E31" t="s">
+        <v>121</v>
+      </c>
+      <c r="F31">
+        <v>52310.9370900473</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="16">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="B32" s="16">
+        <v>99.5</v>
+      </c>
+      <c r="C32" s="16">
+        <f>$F$35*A32^5+$F$34*A32^4+$F$33*A32^3+$F$32*A32^2+$F$31*A32+$F$30</f>
+        <v>99.405541643900506</v>
+      </c>
+      <c r="E32" t="s">
+        <v>122</v>
+      </c>
+      <c r="F32">
+        <v>-29962.807104122399</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="16">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B33" s="16">
+        <v>99</v>
+      </c>
+      <c r="C33" s="16">
+        <f t="shared" ref="C32:C55" si="0">$F$35*A33^5+$F$34*A33^4+$F$33*A33^3+$F$32*A33^2+$F$31*A33+$F$30</f>
+        <v>97.885026838273916</v>
+      </c>
+      <c r="E33" t="s">
+        <v>123</v>
+      </c>
+      <c r="F33">
+        <v>8431.4105127834991</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="16">
+        <v>4.05</v>
+      </c>
+      <c r="B34" s="16">
+        <v>96</v>
+      </c>
+      <c r="C34" s="16">
+        <f t="shared" si="0"/>
+        <v>95.511479702858196</v>
+      </c>
+      <c r="E34" t="s">
+        <v>124</v>
+      </c>
+      <c r="F34">
+        <v>-1164.3507315616</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="16">
+        <v>4</v>
+      </c>
+      <c r="B35" s="16">
+        <v>91</v>
+      </c>
+      <c r="C35" s="16">
+        <f t="shared" si="0"/>
+        <v>92.330696823737526</v>
+      </c>
+      <c r="E35" t="s">
+        <v>125</v>
+      </c>
+      <c r="F35">
+        <v>63.147575745899999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="16">
+        <v>3.95</v>
+      </c>
+      <c r="B36" s="16">
+        <v>87</v>
+      </c>
+      <c r="C36" s="16">
+        <f t="shared" si="0"/>
+        <v>88.405632938047347</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="16">
+        <v>3.9</v>
+      </c>
+      <c r="B37" s="16">
+        <v>83</v>
+      </c>
+      <c r="C37" s="16">
+        <f t="shared" si="0"/>
+        <v>83.814032900780148</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="16">
+        <v>3.85</v>
+      </c>
+      <c r="B38" s="16">
+        <v>78</v>
+      </c>
+      <c r="C38" s="16">
+        <f t="shared" si="0"/>
+        <v>78.646063650106953</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="16">
+        <v>3.8</v>
+      </c>
+      <c r="B39" s="16">
+        <v>73</v>
+      </c>
+      <c r="C39" s="16">
+        <f t="shared" si="0"/>
+        <v>73.001946173659235</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="16">
+        <v>3.75</v>
+      </c>
+      <c r="B40" s="16">
+        <v>67</v>
+      </c>
+      <c r="C40" s="16">
+        <f t="shared" si="0"/>
+        <v>66.989587474461587</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="16">
+        <v>3.7</v>
+      </c>
+      <c r="B41" s="16">
+        <v>62</v>
+      </c>
+      <c r="C41" s="16">
+        <f t="shared" si="0"/>
+        <v>60.722212536311417</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="16">
+        <v>3.65</v>
+      </c>
+      <c r="B42" s="16">
+        <v>57</v>
+      </c>
+      <c r="C42" s="16">
+        <f t="shared" si="0"/>
+        <v>54.315996290177281</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="16">
+        <v>3.6</v>
+      </c>
+      <c r="B43" s="16">
+        <v>50</v>
+      </c>
+      <c r="C43" s="16">
+        <f t="shared" si="0"/>
+        <v>47.887695580277068</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="16">
+        <v>3.55</v>
+      </c>
+      <c r="B44" s="16">
+        <v>43</v>
+      </c>
+      <c r="C44" s="16">
+        <f t="shared" si="0"/>
+        <v>41.55228112925397</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="16">
+        <v>3.5</v>
+      </c>
+      <c r="B45" s="16">
+        <v>36</v>
+      </c>
+      <c r="C45" s="16">
+        <f t="shared" si="0"/>
+        <v>35.420569505040476</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="16">
+        <v>3.45</v>
+      </c>
+      <c r="B46" s="16">
+        <v>28</v>
+      </c>
+      <c r="C46" s="16">
+        <f t="shared" si="0"/>
+        <v>29.596855085597781</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="16">
+        <v>3.4</v>
+      </c>
+      <c r="B47" s="16">
+        <v>21</v>
+      </c>
+      <c r="C47" s="16">
+        <f t="shared" si="0"/>
+        <v>24.176542026129027</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="16">
+        <v>3.35</v>
+      </c>
+      <c r="B48" s="16">
+        <v>17</v>
+      </c>
+      <c r="C48" s="16">
+        <f t="shared" si="0"/>
+        <v>19.243776223993336</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="16">
+        <v>3.3</v>
+      </c>
+      <c r="B49" s="16">
+        <v>13</v>
+      </c>
+      <c r="C49" s="16">
+        <f t="shared" si="0"/>
+        <v>14.869077284987725</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="16">
+        <v>3.25</v>
+      </c>
+      <c r="B50" s="16">
+        <v>10</v>
+      </c>
+      <c r="C50" s="16">
+        <f t="shared" si="0"/>
+        <v>11.106970489425294</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="16">
+        <v>3.2</v>
+      </c>
+      <c r="B51" s="16">
+        <v>8</v>
+      </c>
+      <c r="C51" s="16">
+        <f t="shared" si="0"/>
+        <v>7.9936187574858195</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="16">
+        <v>3.15</v>
+      </c>
+      <c r="B52" s="16">
+        <v>6.5</v>
+      </c>
+      <c r="C52" s="16">
+        <f t="shared" si="0"/>
+        <v>5.5444546161379549</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="16">
+        <v>3.1</v>
+      </c>
+      <c r="B53" s="16">
+        <v>5.4</v>
+      </c>
+      <c r="C53" s="16">
+        <f t="shared" si="0"/>
+        <v>3.7518121635876014</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="16">
+        <v>3.05</v>
+      </c>
+      <c r="B54" s="16">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C54" s="16">
+        <f t="shared" si="0"/>
+        <v>2.5825590366948745</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="16">
+        <v>3</v>
+      </c>
+      <c r="B55" s="16">
+        <v>3.6</v>
+      </c>
+      <c r="C55" s="16">
+        <f t="shared" si="0"/>
+        <v>1.9757283759172424</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="16">
+        <v>2.95</v>
+      </c>
+      <c r="B56" s="16">
+        <v>3</v>
+      </c>
+      <c r="C56" s="16"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="16">
+        <v>2.9</v>
+      </c>
+      <c r="B57" s="16">
+        <v>2.5</v>
+      </c>
+      <c r="C57" s="16"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="16">
+        <v>2.85</v>
+      </c>
+      <c r="B58" s="16">
+        <v>2.1</v>
+      </c>
+      <c r="C58" s="16"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="16">
+        <v>2.8</v>
+      </c>
+      <c r="B59" s="16">
+        <v>1.8</v>
+      </c>
+      <c r="C59" s="16"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="16">
+        <v>2.7500000000000102</v>
+      </c>
+      <c r="B60" s="16">
+        <v>1.5</v>
+      </c>
+      <c r="C60" s="16"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="16">
+        <v>2.7000000000000099</v>
+      </c>
+      <c r="B61" s="16">
+        <v>1.2</v>
+      </c>
+      <c r="C61" s="16"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="16">
+        <v>2.6500000000000101</v>
+      </c>
+      <c r="B62" s="16">
+        <v>1</v>
+      </c>
+      <c r="C62" s="16"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="16">
+        <v>2.6000000000000099</v>
+      </c>
+      <c r="B63" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="C63" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -6777,28 +8748,28 @@
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="32" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="32" t="s">
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="33"/>
-      <c r="P3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="35"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
@@ -6865,10 +8836,10 @@
       <c r="O6" s="25"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="20" t="s">
+      <c r="R6" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="S6" s="20"/>
+      <c r="S6" s="22"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
@@ -6920,18 +8891,18 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20" t="s">
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
@@ -6945,18 +8916,18 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="20">
+      <c r="I9" s="22">
         <v>17</v>
       </c>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20">
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22">
         <v>4</v>
       </c>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
@@ -6975,11 +8946,11 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
-      <c r="N10" s="20" t="s">
+      <c r="N10" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
@@ -6998,24 +8969,18 @@
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
-      <c r="N11" s="21">
+      <c r="N11" s="23">
         <f>100/(2^3-1)*N9</f>
         <v>57.142857142857146</v>
       </c>
-      <c r="O11" s="21"/>
-      <c r="P11" s="21"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="I3:M3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="I6:P6"/>
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="R7:S7"/>
     <mergeCell ref="I8:M8"/>
@@ -7023,6 +8988,12 @@
     <mergeCell ref="I9:M9"/>
     <mergeCell ref="N9:P9"/>
     <mergeCell ref="N10:P10"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="I6:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
sw and hw version updated
</commit_message>
<xml_diff>
--- a/software/BikeCounterPro/src/dataPackage/DataPackage.xlsx
+++ b/software/BikeCounterPro/src/dataPackage/DataPackage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meier\Documents\repos\bikecounter\software\BikeCounterPro\src\dataPackage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D19A1BD-9FD4-432E-8A3D-AE9B35815FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2C24AF-E02A-4084-89CD-9F13CCAA43EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4028" yWindow="1013" windowWidth="13762" windowHeight="10470" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
+    <workbookView xWindow="44796" yWindow="2856" windowWidth="30960" windowHeight="12204" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Data package" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="126">
   <si>
     <t>minutes of day</t>
   </si>
@@ -413,6 +413,9 @@
   </si>
   <si>
     <t>See Tags</t>
+  </si>
+  <si>
+    <t>single board v0.1</t>
   </si>
 </sst>
 </file>
@@ -675,21 +678,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -718,9 +724,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -827,7 +830,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CH"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -910,7 +913,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CH"/>
+                  <a:endParaRPr lang="de-DE"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1043,7 +1046,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CH"/>
+                  <a:endParaRPr lang="de-DE"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1188,7 +1191,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CH"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1627226991"/>
@@ -1251,7 +1254,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CH"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1627225743"/>
@@ -1299,7 +1302,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-CH"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1375,7 +1378,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CH"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1479,7 +1482,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CH"/>
+                  <a:endParaRPr lang="de-DE"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1997,7 +2000,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-CH"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2035,7 +2038,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CH"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="770739263"/>
@@ -2116,7 +2119,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-CH"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2154,7 +2157,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CH"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="637611535"/>
@@ -2207,7 +2210,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-CH"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3408,9 +3411,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3448,7 +3451,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3554,7 +3557,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3696,7 +3699,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3707,18 +3710,18 @@
   <dimension ref="A1:S90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.46484375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.86328125" customWidth="1"/>
-    <col min="5" max="5" width="12.1328125" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -3726,7 +3729,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -3735,12 +3738,12 @@
         <v>408</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -3748,7 +3751,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -3756,7 +3759,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -3765,7 +3768,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>88</v>
       </c>
@@ -3821,7 +3824,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -3833,7 +3836,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -3842,7 +3845,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>89</v>
       </c>
@@ -3898,7 +3901,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -3918,8 +3921,11 @@
       <c r="G17" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="H17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -3940,7 +3946,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
         <v>91</v>
       </c>
@@ -3954,7 +3960,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -3986,7 +3992,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -4001,7 +4007,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -4010,12 +4016,12 @@
         <v>397</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -4038,7 +4044,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -4067,7 +4073,7 @@
         <v>2734992</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -4075,7 +4081,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -4105,7 +4111,7 @@
         <v>3155760</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -4130,7 +4136,7 @@
         <v>420768</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -4155,7 +4161,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
         <v>107</v>
       </c>
@@ -4178,7 +4184,7 @@
         <v>3681648</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E34" t="s">
         <v>102</v>
       </c>
@@ -4199,7 +4205,7 @@
         <v>946656</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -4223,7 +4229,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -4231,7 +4237,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -4239,7 +4245,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -4247,7 +4253,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -4256,7 +4262,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -4266,7 +4272,7 @@
       </c>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -4275,12 +4281,12 @@
         <v>379</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -4288,7 +4294,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -4297,7 +4303,7 @@
         <v>14.285714285714286</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>18</v>
       </c>
@@ -4306,12 +4312,12 @@
         <v>376</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>11</v>
       </c>
@@ -4322,7 +4328,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>109</v>
       </c>
@@ -4337,7 +4343,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>110</v>
       </c>
@@ -4353,7 +4359,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>18</v>
       </c>
@@ -4362,12 +4368,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>11</v>
       </c>
@@ -4375,7 +4381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>18</v>
       </c>
@@ -4384,7 +4390,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="19" t="s">
         <v>4</v>
       </c>
@@ -4394,12 +4400,12 @@
       <c r="E63" s="19"/>
       <c r="F63" s="19"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>1</v>
       </c>
@@ -4414,7 +4420,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>2</v>
       </c>
@@ -4429,7 +4435,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B68">
         <f>2^B67</f>
         <v>2048</v>
@@ -4442,7 +4448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="19" t="s">
         <v>8</v>
       </c>
@@ -4452,7 +4458,7 @@
       <c r="E71" s="19"/>
       <c r="F71" s="19"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -4460,7 +4466,7 @@
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
         <v>51</v>
       </c>
@@ -4470,7 +4476,7 @@
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="7" t="s">
         <v>11</v>
       </c>
@@ -4482,7 +4488,7 @@
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="7" t="s">
         <v>18</v>
       </c>
@@ -4495,13 +4501,13 @@
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>16</v>
       </c>
@@ -4511,7 +4517,7 @@
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>11</v>
       </c>
@@ -4523,7 +4529,7 @@
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>17</v>
       </c>
@@ -4536,7 +4542,7 @@
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -4544,7 +4550,7 @@
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>18</v>
       </c>
@@ -4562,13 +4568,13 @@
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="D82" s="1"/>
       <c r="F82" s="1"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>52</v>
       </c>
@@ -4594,7 +4600,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>0</v>
       </c>
@@ -4625,7 +4631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>1</v>
       </c>
@@ -4656,7 +4662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>2</v>
       </c>
@@ -4687,7 +4693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>3</v>
       </c>
@@ -4718,7 +4724,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>4</v>
       </c>
@@ -4749,10 +4755,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E89" s="3"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E90" s="3"/>
     </row>
   </sheetData>
@@ -4773,55 +4779,55 @@
       <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="32" width="4.19921875" customWidth="1"/>
-    <col min="33" max="150" width="3.1328125" customWidth="1"/>
+    <col min="1" max="32" width="4.21875" customWidth="1"/>
+    <col min="33" max="150" width="3.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="26" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="26" t="s">
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="26" t="s">
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="28"/>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="29"/>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>7</v>
       </c>
@@ -4919,55 +4925,55 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A3" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="32" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="32" t="s">
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="O3" s="33"/>
-      <c r="P3" s="34"/>
-      <c r="Q3" s="32" t="s">
+      <c r="O3" s="34"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="R3" s="33"/>
-      <c r="S3" s="34"/>
-      <c r="T3" s="29" t="s">
+      <c r="R3" s="34"/>
+      <c r="S3" s="35"/>
+      <c r="T3" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="U3" s="30"/>
-      <c r="V3" s="30"/>
-      <c r="W3" s="30"/>
-      <c r="X3" s="31"/>
-      <c r="Y3" s="29" t="s">
+      <c r="U3" s="31"/>
+      <c r="V3" s="31"/>
+      <c r="W3" s="31"/>
+      <c r="X3" s="32"/>
+      <c r="Y3" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="30"/>
-      <c r="AA3" s="30"/>
-      <c r="AB3" s="30"/>
-      <c r="AC3" s="31"/>
-      <c r="AD3" s="29" t="s">
+      <c r="Z3" s="31"/>
+      <c r="AA3" s="31"/>
+      <c r="AB3" s="31"/>
+      <c r="AC3" s="32"/>
+      <c r="AD3" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="AE3" s="30"/>
-      <c r="AF3" s="31"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="AE3" s="31"/>
+      <c r="AF3" s="32"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -4988,7 +4994,7 @@
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
         <v>24</v>
       </c>
@@ -5024,49 +5030,49 @@
       <c r="AE5" s="25"/>
       <c r="AF5" s="25"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A6" s="24" t="s">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A6" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24">
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26">
         <v>38</v>
       </c>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24">
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26">
         <v>73</v>
       </c>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
-      <c r="T6" s="24"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="24"/>
-      <c r="W6" s="24"/>
-      <c r="X6" s="24"/>
-      <c r="Y6" s="24">
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="26"/>
+      <c r="W6" s="26"/>
+      <c r="X6" s="26"/>
+      <c r="Y6" s="26">
         <v>88</v>
       </c>
-      <c r="Z6" s="24"/>
-      <c r="AA6" s="24"/>
-      <c r="AB6" s="24"/>
-      <c r="AC6" s="24"/>
-      <c r="AD6" s="24"/>
-      <c r="AE6" s="24"/>
-      <c r="AF6" s="24"/>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="Z6" s="26"/>
+      <c r="AA6" s="26"/>
+      <c r="AB6" s="26"/>
+      <c r="AC6" s="26"/>
+      <c r="AD6" s="26"/>
+      <c r="AE6" s="26"/>
+      <c r="AF6" s="26"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>0</v>
       </c>
@@ -5164,206 +5170,206 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A8" s="20" t="s">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20" t="s">
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="20" t="s">
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="R8" s="20"/>
-      <c r="S8" s="20"/>
-      <c r="T8" s="20" t="s">
+      <c r="R8" s="22"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="U8" s="20"/>
-      <c r="V8" s="20"/>
-      <c r="W8" s="20"/>
-      <c r="X8" s="20"/>
-      <c r="Y8" s="20" t="s">
+      <c r="U8" s="22"/>
+      <c r="V8" s="22"/>
+      <c r="W8" s="22"/>
+      <c r="X8" s="22"/>
+      <c r="Y8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="Z8" s="20"/>
-      <c r="AA8" s="20"/>
-      <c r="AB8" s="20"/>
-      <c r="AC8" s="20"/>
-      <c r="AD8" s="20" t="s">
+      <c r="Z8" s="22"/>
+      <c r="AA8" s="22"/>
+      <c r="AB8" s="22"/>
+      <c r="AC8" s="22"/>
+      <c r="AD8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="AE8" s="20"/>
-      <c r="AF8" s="20"/>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A9" s="20">
+      <c r="AE8" s="22"/>
+      <c r="AF8" s="22"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A9" s="22">
         <v>10</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20">
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22">
         <v>7</v>
       </c>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20">
-        <v>0</v>
-      </c>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="20">
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22">
+        <v>0</v>
+      </c>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22">
         <v>3</v>
       </c>
-      <c r="R9" s="20"/>
-      <c r="S9" s="20"/>
-      <c r="T9" s="20">
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22">
         <v>19</v>
       </c>
-      <c r="U9" s="20"/>
-      <c r="V9" s="20"/>
-      <c r="W9" s="20"/>
-      <c r="X9" s="20"/>
-      <c r="Y9" s="20">
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22">
         <v>17</v>
       </c>
-      <c r="Z9" s="20"/>
-      <c r="AA9" s="20"/>
-      <c r="AB9" s="20"/>
-      <c r="AC9" s="20"/>
-      <c r="AD9" s="20">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="20"/>
-      <c r="AF9" s="20"/>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A10" s="20" t="s">
+      <c r="Z9" s="22"/>
+      <c r="AA9" s="22"/>
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="22"/>
+      <c r="AD9" s="22">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="22"/>
+      <c r="AF9" s="22"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20" t="s">
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20" t="s">
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="R10" s="20"/>
-      <c r="S10" s="20"/>
-      <c r="T10" s="20" t="s">
+      <c r="R10" s="22"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="U10" s="20"/>
-      <c r="V10" s="20"/>
-      <c r="W10" s="20"/>
-      <c r="X10" s="20"/>
-      <c r="Y10" s="20" t="s">
+      <c r="U10" s="22"/>
+      <c r="V10" s="22"/>
+      <c r="W10" s="22"/>
+      <c r="X10" s="22"/>
+      <c r="Y10" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="Z10" s="20"/>
-      <c r="AA10" s="20"/>
-      <c r="AB10" s="20"/>
-      <c r="AC10" s="20"/>
-      <c r="AD10" s="20" t="s">
+      <c r="Z10" s="22"/>
+      <c r="AA10" s="22"/>
+      <c r="AB10" s="22"/>
+      <c r="AC10" s="22"/>
+      <c r="AD10" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="AE10" s="20"/>
-      <c r="AF10" s="20"/>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A11" s="20">
+      <c r="AE10" s="22"/>
+      <c r="AF10" s="22"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A11" s="22">
         <f>A9</f>
         <v>10</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="21">
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="23">
         <f>'Data package'!$B$31*I9+'Data package'!$B$28</f>
         <v>3.338709677419355</v>
       </c>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="22">
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="20">
         <f ca="1">LOOKUP(N9,'Data package'!$D$21:$D$24,'Data package'!$E$22:$E$35)</f>
         <v>0</v>
       </c>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="23">
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="24">
         <f>100/(2^3-1)*Q9</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23">
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24">
         <f>'Data package'!$B$40*T9+'Data package'!$B$37</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U11" s="22"/>
-      <c r="V11" s="22"/>
-      <c r="W11" s="22"/>
-      <c r="X11" s="22"/>
-      <c r="Y11" s="22">
+      <c r="U11" s="20"/>
+      <c r="V11" s="20"/>
+      <c r="W11" s="20"/>
+      <c r="X11" s="20"/>
+      <c r="Y11" s="20">
         <f>Y9</f>
         <v>17</v>
       </c>
-      <c r="Z11" s="22"/>
-      <c r="AA11" s="22"/>
-      <c r="AB11" s="22"/>
-      <c r="AC11" s="22"/>
-      <c r="AD11" s="22">
+      <c r="Z11" s="20"/>
+      <c r="AA11" s="20"/>
+      <c r="AB11" s="20"/>
+      <c r="AC11" s="20"/>
+      <c r="AD11" s="20">
         <f>LOOKUP(AD9,'Data package'!$A$84:$A$88,'Data package'!$B$84:$B$88)</f>
         <v>1</v>
       </c>
-      <c r="AE11" s="22"/>
-      <c r="AF11" s="22"/>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="AE11" s="20"/>
+      <c r="AF11" s="20"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -5376,7 +5382,7 @@
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
         <v>24</v>
       </c>
@@ -5412,49 +5418,49 @@
       <c r="AE14" s="25"/>
       <c r="AF14" s="25"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A15" s="24" t="s">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A15" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24" t="s">
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24" t="s">
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
-      <c r="U15" s="24"/>
-      <c r="V15" s="24"/>
-      <c r="W15" s="24"/>
-      <c r="X15" s="24"/>
-      <c r="Y15" s="24" t="s">
+      <c r="R15" s="26"/>
+      <c r="S15" s="26"/>
+      <c r="T15" s="26"/>
+      <c r="U15" s="26"/>
+      <c r="V15" s="26"/>
+      <c r="W15" s="26"/>
+      <c r="X15" s="26"/>
+      <c r="Y15" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="Z15" s="24"/>
-      <c r="AA15" s="24"/>
-      <c r="AB15" s="24"/>
-      <c r="AC15" s="24"/>
-      <c r="AD15" s="24"/>
-      <c r="AE15" s="24"/>
-      <c r="AF15" s="24"/>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="Z15" s="26"/>
+      <c r="AA15" s="26"/>
+      <c r="AB15" s="26"/>
+      <c r="AC15" s="26"/>
+      <c r="AD15" s="26"/>
+      <c r="AE15" s="26"/>
+      <c r="AF15" s="26"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>0</v>
       </c>
@@ -5552,206 +5558,206 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:96" x14ac:dyDescent="0.45">
-      <c r="A17" s="20" t="s">
+    <row r="17" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20" t="s">
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="20" t="s">
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="O17" s="20"/>
-      <c r="P17" s="20"/>
-      <c r="Q17" s="20" t="s">
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="R17" s="20"/>
-      <c r="S17" s="20"/>
-      <c r="T17" s="20" t="s">
+      <c r="R17" s="22"/>
+      <c r="S17" s="22"/>
+      <c r="T17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="U17" s="20"/>
-      <c r="V17" s="20"/>
-      <c r="W17" s="20"/>
-      <c r="X17" s="20"/>
-      <c r="Y17" s="20" t="s">
+      <c r="U17" s="22"/>
+      <c r="V17" s="22"/>
+      <c r="W17" s="22"/>
+      <c r="X17" s="22"/>
+      <c r="Y17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="Z17" s="20"/>
-      <c r="AA17" s="20"/>
-      <c r="AB17" s="20"/>
-      <c r="AC17" s="20"/>
-      <c r="AD17" s="20" t="s">
+      <c r="Z17" s="22"/>
+      <c r="AA17" s="22"/>
+      <c r="AB17" s="22"/>
+      <c r="AC17" s="22"/>
+      <c r="AD17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="AE17" s="20"/>
-      <c r="AF17" s="20"/>
-    </row>
-    <row r="18" spans="1:96" x14ac:dyDescent="0.45">
-      <c r="A18" s="20">
+      <c r="AE17" s="22"/>
+      <c r="AF17" s="22"/>
+    </row>
+    <row r="18" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A18" s="22">
         <v>5</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20">
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22">
         <v>8</v>
       </c>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20">
-        <v>0</v>
-      </c>
-      <c r="O18" s="20"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="20">
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22">
+        <v>0</v>
+      </c>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22">
         <v>3</v>
       </c>
-      <c r="R18" s="20"/>
-      <c r="S18" s="20"/>
-      <c r="T18" s="20">
+      <c r="R18" s="22"/>
+      <c r="S18" s="22"/>
+      <c r="T18" s="22">
         <v>19</v>
       </c>
-      <c r="U18" s="20"/>
-      <c r="V18" s="20"/>
-      <c r="W18" s="20"/>
-      <c r="X18" s="20"/>
-      <c r="Y18" s="20">
+      <c r="U18" s="22"/>
+      <c r="V18" s="22"/>
+      <c r="W18" s="22"/>
+      <c r="X18" s="22"/>
+      <c r="Y18" s="22">
         <v>17</v>
       </c>
-      <c r="Z18" s="20"/>
-      <c r="AA18" s="20"/>
-      <c r="AB18" s="20"/>
-      <c r="AC18" s="20"/>
-      <c r="AD18" s="20">
-        <v>0</v>
-      </c>
-      <c r="AE18" s="20"/>
-      <c r="AF18" s="20"/>
-    </row>
-    <row r="19" spans="1:96" x14ac:dyDescent="0.45">
-      <c r="A19" s="20" t="s">
+      <c r="Z18" s="22"/>
+      <c r="AA18" s="22"/>
+      <c r="AB18" s="22"/>
+      <c r="AC18" s="22"/>
+      <c r="AD18" s="22">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="22"/>
+      <c r="AF18" s="22"/>
+    </row>
+    <row r="19" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A19" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20" t="s">
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="20" t="s">
+      <c r="O19" s="22"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="R19" s="20"/>
-      <c r="S19" s="20"/>
-      <c r="T19" s="20" t="s">
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
+      <c r="T19" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="U19" s="20"/>
-      <c r="V19" s="20"/>
-      <c r="W19" s="20"/>
-      <c r="X19" s="20"/>
-      <c r="Y19" s="20" t="s">
+      <c r="U19" s="22"/>
+      <c r="V19" s="22"/>
+      <c r="W19" s="22"/>
+      <c r="X19" s="22"/>
+      <c r="Y19" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="Z19" s="20"/>
-      <c r="AA19" s="20"/>
-      <c r="AB19" s="20"/>
-      <c r="AC19" s="20"/>
-      <c r="AD19" s="20" t="s">
+      <c r="Z19" s="22"/>
+      <c r="AA19" s="22"/>
+      <c r="AB19" s="22"/>
+      <c r="AC19" s="22"/>
+      <c r="AD19" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="AE19" s="20"/>
-      <c r="AF19" s="20"/>
-    </row>
-    <row r="20" spans="1:96" x14ac:dyDescent="0.45">
-      <c r="A20" s="20">
+      <c r="AE19" s="22"/>
+      <c r="AF19" s="22"/>
+    </row>
+    <row r="20" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A20" s="22">
         <f>A18</f>
         <v>5</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="21">
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="23">
         <f>'Data package'!$B$31*I18+'Data package'!$B$28</f>
         <v>3.3870967741935485</v>
       </c>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="22">
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="20">
         <f ca="1">LOOKUP(N18,'Data package'!$D$21:$D$24,'Data package'!$E$22:$E$35)</f>
         <v>0</v>
       </c>
-      <c r="O20" s="22"/>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="23">
+      <c r="O20" s="20"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="24">
         <f>100/(2^3-1)*Q18</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R20" s="23"/>
-      <c r="S20" s="23"/>
-      <c r="T20" s="23">
+      <c r="R20" s="24"/>
+      <c r="S20" s="24"/>
+      <c r="T20" s="24">
         <f>'Data package'!$B$40*T18+'Data package'!$B$37</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U20" s="22"/>
-      <c r="V20" s="22"/>
-      <c r="W20" s="22"/>
-      <c r="X20" s="22"/>
-      <c r="Y20" s="22">
+      <c r="U20" s="20"/>
+      <c r="V20" s="20"/>
+      <c r="W20" s="20"/>
+      <c r="X20" s="20"/>
+      <c r="Y20" s="20">
         <f>Y18</f>
         <v>17</v>
       </c>
-      <c r="Z20" s="22"/>
-      <c r="AA20" s="22"/>
-      <c r="AB20" s="22"/>
-      <c r="AC20" s="22"/>
-      <c r="AD20" s="22">
+      <c r="Z20" s="20"/>
+      <c r="AA20" s="20"/>
+      <c r="AB20" s="20"/>
+      <c r="AC20" s="20"/>
+      <c r="AD20" s="20">
         <f>LOOKUP(AD18,'Data package'!$A$84:$A$88,'Data package'!$B$84:$B$88)</f>
         <v>1</v>
       </c>
-      <c r="AE20" s="22"/>
-      <c r="AF20" s="22"/>
-    </row>
-    <row r="23" spans="1:96" x14ac:dyDescent="0.45">
+      <c r="AE20" s="20"/>
+      <c r="AF20" s="20"/>
+    </row>
+    <row r="23" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A23" s="25" t="s">
         <v>24</v>
       </c>
@@ -5787,129 +5793,129 @@
       <c r="AE23" s="25"/>
       <c r="AF23" s="25"/>
     </row>
-    <row r="24" spans="1:96" x14ac:dyDescent="0.45">
-      <c r="A24" s="24" t="s">
+    <row r="24" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A24" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24" t="s">
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="24"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="24"/>
-      <c r="Q24" s="24" t="s">
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="26"/>
+      <c r="Q24" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="R24" s="24"/>
-      <c r="S24" s="24"/>
-      <c r="T24" s="24"/>
-      <c r="U24" s="24"/>
-      <c r="V24" s="24"/>
-      <c r="W24" s="24"/>
-      <c r="X24" s="24"/>
-      <c r="Y24" s="24" t="s">
+      <c r="R24" s="26"/>
+      <c r="S24" s="26"/>
+      <c r="T24" s="26"/>
+      <c r="U24" s="26"/>
+      <c r="V24" s="26"/>
+      <c r="W24" s="26"/>
+      <c r="X24" s="26"/>
+      <c r="Y24" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="Z24" s="24"/>
-      <c r="AA24" s="24"/>
-      <c r="AB24" s="24"/>
-      <c r="AC24" s="24"/>
-      <c r="AD24" s="24"/>
-      <c r="AE24" s="24"/>
-      <c r="AF24" s="24"/>
-      <c r="AG24" s="35">
+      <c r="Z24" s="26"/>
+      <c r="AA24" s="26"/>
+      <c r="AB24" s="26"/>
+      <c r="AC24" s="26"/>
+      <c r="AD24" s="26"/>
+      <c r="AE24" s="26"/>
+      <c r="AF24" s="26"/>
+      <c r="AG24" s="21">
         <v>59</v>
       </c>
-      <c r="AH24" s="35"/>
-      <c r="AI24" s="35"/>
-      <c r="AJ24" s="35"/>
-      <c r="AK24" s="35"/>
-      <c r="AL24" s="35"/>
-      <c r="AM24" s="35"/>
-      <c r="AN24" s="35"/>
-      <c r="AO24" s="35">
+      <c r="AH24" s="21"/>
+      <c r="AI24" s="21"/>
+      <c r="AJ24" s="21"/>
+      <c r="AK24" s="21"/>
+      <c r="AL24" s="21"/>
+      <c r="AM24" s="21"/>
+      <c r="AN24" s="21"/>
+      <c r="AO24" s="21">
         <v>96</v>
       </c>
-      <c r="AP24" s="35"/>
-      <c r="AQ24" s="35"/>
-      <c r="AR24" s="35"/>
-      <c r="AS24" s="35"/>
-      <c r="AT24" s="35"/>
-      <c r="AU24" s="35"/>
-      <c r="AV24" s="35"/>
-      <c r="AW24" s="35">
+      <c r="AP24" s="21"/>
+      <c r="AQ24" s="21"/>
+      <c r="AR24" s="21"/>
+      <c r="AS24" s="21"/>
+      <c r="AT24" s="21"/>
+      <c r="AU24" s="21"/>
+      <c r="AV24" s="21"/>
+      <c r="AW24" s="21">
         <v>65</v>
       </c>
-      <c r="AX24" s="35"/>
-      <c r="AY24" s="35"/>
-      <c r="AZ24" s="35"/>
-      <c r="BA24" s="35"/>
-      <c r="BB24" s="35"/>
-      <c r="BC24" s="35"/>
-      <c r="BD24" s="35"/>
-      <c r="BE24" s="35" t="s">
+      <c r="AX24" s="21"/>
+      <c r="AY24" s="21"/>
+      <c r="AZ24" s="21"/>
+      <c r="BA24" s="21"/>
+      <c r="BB24" s="21"/>
+      <c r="BC24" s="21"/>
+      <c r="BD24" s="21"/>
+      <c r="BE24" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="BF24" s="35"/>
-      <c r="BG24" s="35"/>
-      <c r="BH24" s="35"/>
-      <c r="BI24" s="35"/>
-      <c r="BJ24" s="35"/>
-      <c r="BK24" s="35"/>
-      <c r="BL24" s="35"/>
-      <c r="BM24" s="35" t="s">
+      <c r="BF24" s="21"/>
+      <c r="BG24" s="21"/>
+      <c r="BH24" s="21"/>
+      <c r="BI24" s="21"/>
+      <c r="BJ24" s="21"/>
+      <c r="BK24" s="21"/>
+      <c r="BL24" s="21"/>
+      <c r="BM24" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="BN24" s="35"/>
-      <c r="BO24" s="35"/>
-      <c r="BP24" s="35"/>
-      <c r="BQ24" s="35"/>
-      <c r="BR24" s="35"/>
-      <c r="BS24" s="35"/>
-      <c r="BT24" s="35"/>
-      <c r="BU24" s="35">
+      <c r="BN24" s="21"/>
+      <c r="BO24" s="21"/>
+      <c r="BP24" s="21"/>
+      <c r="BQ24" s="21"/>
+      <c r="BR24" s="21"/>
+      <c r="BS24" s="21"/>
+      <c r="BT24" s="21"/>
+      <c r="BU24" s="21">
         <v>69</v>
       </c>
-      <c r="BV24" s="35"/>
-      <c r="BW24" s="35"/>
-      <c r="BX24" s="35"/>
-      <c r="BY24" s="35"/>
-      <c r="BZ24" s="35"/>
-      <c r="CA24" s="35"/>
-      <c r="CB24" s="35"/>
-      <c r="CC24" s="35" t="s">
+      <c r="BV24" s="21"/>
+      <c r="BW24" s="21"/>
+      <c r="BX24" s="21"/>
+      <c r="BY24" s="21"/>
+      <c r="BZ24" s="21"/>
+      <c r="CA24" s="21"/>
+      <c r="CB24" s="21"/>
+      <c r="CC24" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="CD24" s="35"/>
-      <c r="CE24" s="35"/>
-      <c r="CF24" s="35"/>
-      <c r="CG24" s="35"/>
-      <c r="CH24" s="35"/>
-      <c r="CI24" s="35"/>
-      <c r="CJ24" s="35"/>
-      <c r="CK24" s="35" t="s">
+      <c r="CD24" s="21"/>
+      <c r="CE24" s="21"/>
+      <c r="CF24" s="21"/>
+      <c r="CG24" s="21"/>
+      <c r="CH24" s="21"/>
+      <c r="CI24" s="21"/>
+      <c r="CJ24" s="21"/>
+      <c r="CK24" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="CL24" s="35"/>
-      <c r="CM24" s="35"/>
-      <c r="CN24" s="35"/>
-      <c r="CO24" s="35"/>
-      <c r="CP24" s="35"/>
-      <c r="CQ24" s="35"/>
-      <c r="CR24" s="35"/>
-    </row>
-    <row r="25" spans="1:96" x14ac:dyDescent="0.45">
+      <c r="CL24" s="21"/>
+      <c r="CM24" s="21"/>
+      <c r="CN24" s="21"/>
+      <c r="CO24" s="21"/>
+      <c r="CP24" s="21"/>
+      <c r="CQ24" s="21"/>
+      <c r="CR24" s="21"/>
+    </row>
+    <row r="25" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>0</v>
       </c>
@@ -6199,181 +6205,181 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:96" x14ac:dyDescent="0.45">
-      <c r="A26" s="20" t="s">
+    <row r="26" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20" t="s">
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20" t="s">
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="O26" s="20"/>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="20" t="s">
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="R26" s="20"/>
-      <c r="S26" s="20"/>
-      <c r="T26" s="20" t="s">
+      <c r="R26" s="22"/>
+      <c r="S26" s="22"/>
+      <c r="T26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="U26" s="20"/>
-      <c r="V26" s="20"/>
-      <c r="W26" s="20"/>
-      <c r="X26" s="20"/>
-      <c r="Y26" s="20" t="s">
+      <c r="U26" s="22"/>
+      <c r="V26" s="22"/>
+      <c r="W26" s="22"/>
+      <c r="X26" s="22"/>
+      <c r="Y26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="Z26" s="20"/>
-      <c r="AA26" s="20"/>
-      <c r="AB26" s="20"/>
-      <c r="AC26" s="20"/>
-      <c r="AD26" s="20" t="s">
+      <c r="Z26" s="22"/>
+      <c r="AA26" s="22"/>
+      <c r="AB26" s="22"/>
+      <c r="AC26" s="22"/>
+      <c r="AD26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="AE26" s="20"/>
-      <c r="AF26" s="20"/>
-      <c r="AG26" s="22" t="s">
+      <c r="AE26" s="22"/>
+      <c r="AF26" s="22"/>
+      <c r="AG26" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AH26" s="22"/>
-      <c r="AI26" s="22"/>
-      <c r="AJ26" s="22"/>
-      <c r="AK26" s="22"/>
-      <c r="AL26" s="22"/>
-      <c r="AM26" s="22"/>
-      <c r="AN26" s="22"/>
-      <c r="AO26" s="22" t="s">
+      <c r="AH26" s="20"/>
+      <c r="AI26" s="20"/>
+      <c r="AJ26" s="20"/>
+      <c r="AK26" s="20"/>
+      <c r="AL26" s="20"/>
+      <c r="AM26" s="20"/>
+      <c r="AN26" s="20"/>
+      <c r="AO26" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AP26" s="22"/>
-      <c r="AQ26" s="22"/>
-      <c r="AR26" s="22"/>
-      <c r="AS26" s="22"/>
-      <c r="AT26" s="22"/>
-      <c r="AU26" s="22"/>
-      <c r="AV26" s="22"/>
-      <c r="AW26" s="22" t="s">
+      <c r="AP26" s="20"/>
+      <c r="AQ26" s="20"/>
+      <c r="AR26" s="20"/>
+      <c r="AS26" s="20"/>
+      <c r="AT26" s="20"/>
+      <c r="AU26" s="20"/>
+      <c r="AV26" s="20"/>
+      <c r="AW26" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AX26" s="22"/>
-      <c r="AY26" s="22"/>
-      <c r="AZ26" s="22"/>
-      <c r="BA26" s="22"/>
-      <c r="BB26" s="22"/>
-      <c r="BC26" s="22"/>
-      <c r="BD26" s="22"/>
-      <c r="BE26" s="22" t="s">
+      <c r="AX26" s="20"/>
+      <c r="AY26" s="20"/>
+      <c r="AZ26" s="20"/>
+      <c r="BA26" s="20"/>
+      <c r="BB26" s="20"/>
+      <c r="BC26" s="20"/>
+      <c r="BD26" s="20"/>
+      <c r="BE26" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="BF26" s="22"/>
-      <c r="BG26" s="22"/>
-      <c r="BH26" s="22"/>
-      <c r="BI26" s="22"/>
-      <c r="BJ26" s="22"/>
-      <c r="BK26" s="22"/>
-      <c r="BL26" s="22"/>
-      <c r="BM26" s="22" t="s">
+      <c r="BF26" s="20"/>
+      <c r="BG26" s="20"/>
+      <c r="BH26" s="20"/>
+      <c r="BI26" s="20"/>
+      <c r="BJ26" s="20"/>
+      <c r="BK26" s="20"/>
+      <c r="BL26" s="20"/>
+      <c r="BM26" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="BN26" s="22"/>
-      <c r="BO26" s="22"/>
-      <c r="BP26" s="22"/>
-      <c r="BQ26" s="22"/>
-      <c r="BR26" s="22"/>
-      <c r="BS26" s="22"/>
-      <c r="BT26" s="22"/>
-      <c r="BU26" s="22" t="s">
+      <c r="BN26" s="20"/>
+      <c r="BO26" s="20"/>
+      <c r="BP26" s="20"/>
+      <c r="BQ26" s="20"/>
+      <c r="BR26" s="20"/>
+      <c r="BS26" s="20"/>
+      <c r="BT26" s="20"/>
+      <c r="BU26" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="BV26" s="22"/>
-      <c r="BW26" s="22"/>
-      <c r="BX26" s="22"/>
-      <c r="BY26" s="22"/>
-      <c r="BZ26" s="22"/>
-      <c r="CA26" s="22"/>
-      <c r="CB26" s="22"/>
-      <c r="CC26" s="22" t="s">
+      <c r="BV26" s="20"/>
+      <c r="BW26" s="20"/>
+      <c r="BX26" s="20"/>
+      <c r="BY26" s="20"/>
+      <c r="BZ26" s="20"/>
+      <c r="CA26" s="20"/>
+      <c r="CB26" s="20"/>
+      <c r="CC26" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="CD26" s="22"/>
-      <c r="CE26" s="22"/>
-      <c r="CF26" s="22"/>
-      <c r="CG26" s="22"/>
-      <c r="CH26" s="22"/>
-      <c r="CI26" s="22"/>
-      <c r="CJ26" s="22"/>
-      <c r="CK26" s="22" t="s">
+      <c r="CD26" s="20"/>
+      <c r="CE26" s="20"/>
+      <c r="CF26" s="20"/>
+      <c r="CG26" s="20"/>
+      <c r="CH26" s="20"/>
+      <c r="CI26" s="20"/>
+      <c r="CJ26" s="20"/>
+      <c r="CK26" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="CL26" s="22"/>
-      <c r="CM26" s="22"/>
-      <c r="CN26" s="22"/>
-      <c r="CO26" s="22"/>
-      <c r="CP26" s="22"/>
-      <c r="CQ26" s="22"/>
-      <c r="CR26" s="22"/>
-    </row>
-    <row r="27" spans="1:96" x14ac:dyDescent="0.45">
-      <c r="A27" s="20">
+      <c r="CL26" s="20"/>
+      <c r="CM26" s="20"/>
+      <c r="CN26" s="20"/>
+      <c r="CO26" s="20"/>
+      <c r="CP26" s="20"/>
+      <c r="CQ26" s="20"/>
+      <c r="CR26" s="20"/>
+    </row>
+    <row r="27" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A27" s="22">
         <v>10</v>
       </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20">
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22">
         <v>8</v>
       </c>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20">
-        <v>0</v>
-      </c>
-      <c r="O27" s="20"/>
-      <c r="P27" s="20"/>
-      <c r="Q27" s="20">
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22">
+        <v>0</v>
+      </c>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22">
         <v>3</v>
       </c>
-      <c r="R27" s="20"/>
-      <c r="S27" s="20"/>
-      <c r="T27" s="20">
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="22">
         <v>19</v>
       </c>
-      <c r="U27" s="20"/>
-      <c r="V27" s="20"/>
-      <c r="W27" s="20"/>
-      <c r="X27" s="20"/>
-      <c r="Y27" s="20">
+      <c r="U27" s="22"/>
+      <c r="V27" s="22"/>
+      <c r="W27" s="22"/>
+      <c r="X27" s="22"/>
+      <c r="Y27" s="22">
         <v>21</v>
       </c>
-      <c r="Z27" s="20"/>
-      <c r="AA27" s="20"/>
-      <c r="AB27" s="20"/>
-      <c r="AC27" s="20"/>
-      <c r="AD27" s="20">
-        <v>0</v>
-      </c>
-      <c r="AE27" s="20"/>
-      <c r="AF27" s="20"/>
+      <c r="Z27" s="22"/>
+      <c r="AA27" s="22"/>
+      <c r="AB27" s="22"/>
+      <c r="AC27" s="22"/>
+      <c r="AD27" s="22">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="22"/>
+      <c r="AF27" s="22"/>
       <c r="AG27">
         <f>AN25</f>
         <v>1</v>
@@ -6631,270 +6637,270 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:96" x14ac:dyDescent="0.45">
-      <c r="A28" s="20" t="s">
+    <row r="28" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A28" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20" t="s">
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="20"/>
-      <c r="M28" s="20"/>
-      <c r="N28" s="20" t="s">
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="O28" s="20"/>
-      <c r="P28" s="20"/>
-      <c r="Q28" s="20" t="s">
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="R28" s="20"/>
-      <c r="S28" s="20"/>
-      <c r="T28" s="20" t="s">
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="U28" s="20"/>
-      <c r="V28" s="20"/>
-      <c r="W28" s="20"/>
-      <c r="X28" s="20"/>
-      <c r="Y28" s="20" t="s">
+      <c r="U28" s="22"/>
+      <c r="V28" s="22"/>
+      <c r="W28" s="22"/>
+      <c r="X28" s="22"/>
+      <c r="Y28" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="Z28" s="20"/>
-      <c r="AA28" s="20"/>
-      <c r="AB28" s="20"/>
-      <c r="AC28" s="20"/>
-      <c r="AD28" s="20" t="s">
+      <c r="Z28" s="22"/>
+      <c r="AA28" s="22"/>
+      <c r="AB28" s="22"/>
+      <c r="AC28" s="22"/>
+      <c r="AD28" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="AE28" s="20"/>
-      <c r="AF28" s="20"/>
-      <c r="AG28" s="22" t="s">
+      <c r="AE28" s="22"/>
+      <c r="AF28" s="22"/>
+      <c r="AG28" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="AH28" s="22"/>
-      <c r="AI28" s="22"/>
-      <c r="AJ28" s="22"/>
-      <c r="AK28" s="22"/>
-      <c r="AL28" s="22"/>
-      <c r="AM28" s="22" t="s">
+      <c r="AH28" s="20"/>
+      <c r="AI28" s="20"/>
+      <c r="AJ28" s="20"/>
+      <c r="AK28" s="20"/>
+      <c r="AL28" s="20"/>
+      <c r="AM28" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="AN28" s="22"/>
-      <c r="AO28" s="22"/>
-      <c r="AP28" s="22"/>
-      <c r="AQ28" s="22"/>
-      <c r="AR28" s="22"/>
-      <c r="AS28" s="22" t="s">
+      <c r="AN28" s="20"/>
+      <c r="AO28" s="20"/>
+      <c r="AP28" s="20"/>
+      <c r="AQ28" s="20"/>
+      <c r="AR28" s="20"/>
+      <c r="AS28" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="AT28" s="22"/>
-      <c r="AU28" s="22"/>
-      <c r="AV28" s="22"/>
-      <c r="AW28" s="22"/>
-      <c r="AX28" s="22"/>
-      <c r="AY28" s="22" t="s">
+      <c r="AT28" s="20"/>
+      <c r="AU28" s="20"/>
+      <c r="AV28" s="20"/>
+      <c r="AW28" s="20"/>
+      <c r="AX28" s="20"/>
+      <c r="AY28" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="AZ28" s="22"/>
-      <c r="BA28" s="22"/>
-      <c r="BB28" s="22"/>
-      <c r="BC28" s="22"/>
-      <c r="BD28" s="22"/>
-      <c r="BE28" s="22" t="s">
+      <c r="AZ28" s="20"/>
+      <c r="BA28" s="20"/>
+      <c r="BB28" s="20"/>
+      <c r="BC28" s="20"/>
+      <c r="BD28" s="20"/>
+      <c r="BE28" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="BF28" s="22"/>
-      <c r="BG28" s="22"/>
-      <c r="BH28" s="22"/>
-      <c r="BI28" s="22"/>
-      <c r="BJ28" s="22"/>
-      <c r="BK28" s="22" t="s">
+      <c r="BF28" s="20"/>
+      <c r="BG28" s="20"/>
+      <c r="BH28" s="20"/>
+      <c r="BI28" s="20"/>
+      <c r="BJ28" s="20"/>
+      <c r="BK28" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="BL28" s="22"/>
-      <c r="BM28" s="22"/>
-      <c r="BN28" s="22"/>
-      <c r="BO28" s="22"/>
-      <c r="BP28" s="22"/>
-      <c r="BQ28" s="22" t="s">
+      <c r="BL28" s="20"/>
+      <c r="BM28" s="20"/>
+      <c r="BN28" s="20"/>
+      <c r="BO28" s="20"/>
+      <c r="BP28" s="20"/>
+      <c r="BQ28" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="BR28" s="22"/>
-      <c r="BS28" s="22"/>
-      <c r="BT28" s="22"/>
-      <c r="BU28" s="22"/>
-      <c r="BV28" s="22"/>
-      <c r="BW28" s="22" t="s">
+      <c r="BR28" s="20"/>
+      <c r="BS28" s="20"/>
+      <c r="BT28" s="20"/>
+      <c r="BU28" s="20"/>
+      <c r="BV28" s="20"/>
+      <c r="BW28" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="BX28" s="22"/>
-      <c r="BY28" s="22"/>
-      <c r="BZ28" s="22"/>
-      <c r="CA28" s="22"/>
-      <c r="CB28" s="22"/>
-      <c r="CC28" s="22" t="s">
+      <c r="BX28" s="20"/>
+      <c r="BY28" s="20"/>
+      <c r="BZ28" s="20"/>
+      <c r="CA28" s="20"/>
+      <c r="CB28" s="20"/>
+      <c r="CC28" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="CD28" s="22"/>
-      <c r="CE28" s="22"/>
-      <c r="CF28" s="22"/>
-      <c r="CG28" s="22"/>
-      <c r="CH28" s="22"/>
-      <c r="CI28" s="22" t="s">
+      <c r="CD28" s="20"/>
+      <c r="CE28" s="20"/>
+      <c r="CF28" s="20"/>
+      <c r="CG28" s="20"/>
+      <c r="CH28" s="20"/>
+      <c r="CI28" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="CJ28" s="22"/>
-      <c r="CK28" s="22"/>
-      <c r="CL28" s="22"/>
-      <c r="CM28" s="22"/>
-      <c r="CN28" s="22"/>
-    </row>
-    <row r="29" spans="1:96" x14ac:dyDescent="0.45">
-      <c r="A29" s="20">
+      <c r="CJ28" s="20"/>
+      <c r="CK28" s="20"/>
+      <c r="CL28" s="20"/>
+      <c r="CM28" s="20"/>
+      <c r="CN28" s="20"/>
+    </row>
+    <row r="29" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A29" s="22">
         <f>A27</f>
         <v>10</v>
       </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="21">
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="23">
         <f>'Data package'!$B$31*I27+'Data package'!$B$28</f>
         <v>3.3870967741935485</v>
       </c>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="21"/>
-      <c r="M29" s="21"/>
-      <c r="N29" s="22">
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="20">
         <f ca="1">LOOKUP(N27,'Data package'!$D$21:$D$24,'Data package'!$E$22:$E$35)</f>
         <v>0</v>
       </c>
-      <c r="O29" s="22"/>
-      <c r="P29" s="22"/>
-      <c r="Q29" s="23">
+      <c r="O29" s="20"/>
+      <c r="P29" s="20"/>
+      <c r="Q29" s="24">
         <f>100/(2^3-1)*Q27</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R29" s="23"/>
-      <c r="S29" s="23"/>
-      <c r="T29" s="23">
+      <c r="R29" s="24"/>
+      <c r="S29" s="24"/>
+      <c r="T29" s="24">
         <f>'Data package'!$B$40*T27+'Data package'!$B$37</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U29" s="22"/>
-      <c r="V29" s="22"/>
-      <c r="W29" s="22"/>
-      <c r="X29" s="22"/>
-      <c r="Y29" s="22">
+      <c r="U29" s="20"/>
+      <c r="V29" s="20"/>
+      <c r="W29" s="20"/>
+      <c r="X29" s="20"/>
+      <c r="Y29" s="20">
         <f>Y27</f>
         <v>21</v>
       </c>
-      <c r="Z29" s="22"/>
-      <c r="AA29" s="22"/>
-      <c r="AB29" s="22"/>
-      <c r="AC29" s="22"/>
-      <c r="AD29" s="22">
+      <c r="Z29" s="20"/>
+      <c r="AA29" s="20"/>
+      <c r="AB29" s="20"/>
+      <c r="AC29" s="20"/>
+      <c r="AD29" s="20">
         <f>LOOKUP(AD27,'Data package'!$A$84:$A$88,'Data package'!$B$84:$B$88)</f>
         <v>1</v>
       </c>
-      <c r="AE29" s="22"/>
-      <c r="AF29" s="22"/>
-      <c r="AG29" s="22" t="s">
+      <c r="AE29" s="20"/>
+      <c r="AF29" s="20"/>
+      <c r="AG29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AH29" s="22"/>
-      <c r="AI29" s="22"/>
-      <c r="AJ29" s="22"/>
-      <c r="AK29" s="22"/>
-      <c r="AL29" s="22"/>
-      <c r="AM29" s="22" t="s">
+      <c r="AH29" s="20"/>
+      <c r="AI29" s="20"/>
+      <c r="AJ29" s="20"/>
+      <c r="AK29" s="20"/>
+      <c r="AL29" s="20"/>
+      <c r="AM29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AN29" s="22"/>
-      <c r="AO29" s="22"/>
-      <c r="AP29" s="22"/>
-      <c r="AQ29" s="22"/>
-      <c r="AR29" s="22"/>
-      <c r="AS29" s="22" t="s">
+      <c r="AN29" s="20"/>
+      <c r="AO29" s="20"/>
+      <c r="AP29" s="20"/>
+      <c r="AQ29" s="20"/>
+      <c r="AR29" s="20"/>
+      <c r="AS29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AT29" s="22"/>
-      <c r="AU29" s="22"/>
-      <c r="AV29" s="22"/>
-      <c r="AW29" s="22"/>
-      <c r="AX29" s="22"/>
-      <c r="AY29" s="22" t="s">
+      <c r="AT29" s="20"/>
+      <c r="AU29" s="20"/>
+      <c r="AV29" s="20"/>
+      <c r="AW29" s="20"/>
+      <c r="AX29" s="20"/>
+      <c r="AY29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AZ29" s="22"/>
-      <c r="BA29" s="22"/>
-      <c r="BB29" s="22"/>
-      <c r="BC29" s="22"/>
-      <c r="BD29" s="22"/>
-      <c r="BE29" s="22" t="s">
+      <c r="AZ29" s="20"/>
+      <c r="BA29" s="20"/>
+      <c r="BB29" s="20"/>
+      <c r="BC29" s="20"/>
+      <c r="BD29" s="20"/>
+      <c r="BE29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="BF29" s="22"/>
-      <c r="BG29" s="22"/>
-      <c r="BH29" s="22"/>
-      <c r="BI29" s="22"/>
-      <c r="BJ29" s="22"/>
-      <c r="BK29" s="22" t="s">
+      <c r="BF29" s="20"/>
+      <c r="BG29" s="20"/>
+      <c r="BH29" s="20"/>
+      <c r="BI29" s="20"/>
+      <c r="BJ29" s="20"/>
+      <c r="BK29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="BL29" s="22"/>
-      <c r="BM29" s="22"/>
-      <c r="BN29" s="22"/>
-      <c r="BO29" s="22"/>
-      <c r="BP29" s="22"/>
-      <c r="BQ29" s="22" t="s">
+      <c r="BL29" s="20"/>
+      <c r="BM29" s="20"/>
+      <c r="BN29" s="20"/>
+      <c r="BO29" s="20"/>
+      <c r="BP29" s="20"/>
+      <c r="BQ29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="BR29" s="22"/>
-      <c r="BS29" s="22"/>
-      <c r="BT29" s="22"/>
-      <c r="BU29" s="22"/>
-      <c r="BV29" s="22"/>
-      <c r="BW29" s="22" t="s">
+      <c r="BR29" s="20"/>
+      <c r="BS29" s="20"/>
+      <c r="BT29" s="20"/>
+      <c r="BU29" s="20"/>
+      <c r="BV29" s="20"/>
+      <c r="BW29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="BX29" s="22"/>
-      <c r="BY29" s="22"/>
-      <c r="BZ29" s="22"/>
-      <c r="CA29" s="22"/>
-      <c r="CB29" s="22"/>
-      <c r="CC29" s="22" t="s">
+      <c r="BX29" s="20"/>
+      <c r="BY29" s="20"/>
+      <c r="BZ29" s="20"/>
+      <c r="CA29" s="20"/>
+      <c r="CB29" s="20"/>
+      <c r="CC29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="CD29" s="22"/>
-      <c r="CE29" s="22"/>
-      <c r="CF29" s="22"/>
-      <c r="CG29" s="22"/>
-      <c r="CH29" s="22"/>
-      <c r="CI29" s="22" t="s">
+      <c r="CD29" s="20"/>
+      <c r="CE29" s="20"/>
+      <c r="CF29" s="20"/>
+      <c r="CG29" s="20"/>
+      <c r="CH29" s="20"/>
+      <c r="CI29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="CJ29" s="22"/>
-      <c r="CK29" s="22"/>
-      <c r="CL29" s="22"/>
-      <c r="CM29" s="22"/>
-      <c r="CN29" s="22"/>
-    </row>
-    <row r="30" spans="1:96" x14ac:dyDescent="0.45">
+      <c r="CJ29" s="20"/>
+      <c r="CK29" s="20"/>
+      <c r="CL29" s="20"/>
+      <c r="CM29" s="20"/>
+      <c r="CN29" s="20"/>
+    </row>
+    <row r="30" spans="1:96" x14ac:dyDescent="0.3">
       <c r="AG30">
         <f>AL27</f>
         <v>0</v>
@@ -7136,256 +7142,230 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:96" x14ac:dyDescent="0.45">
-      <c r="AG31" s="22" t="s">
+    <row r="31" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="AG31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="AH31" s="22"/>
-      <c r="AI31" s="22"/>
-      <c r="AJ31" s="22"/>
-      <c r="AK31" s="22"/>
-      <c r="AL31" s="22"/>
-      <c r="AM31" s="22" t="s">
+      <c r="AH31" s="20"/>
+      <c r="AI31" s="20"/>
+      <c r="AJ31" s="20"/>
+      <c r="AK31" s="20"/>
+      <c r="AL31" s="20"/>
+      <c r="AM31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="AN31" s="22"/>
-      <c r="AO31" s="22"/>
-      <c r="AP31" s="22"/>
-      <c r="AQ31" s="22"/>
-      <c r="AR31" s="22"/>
-      <c r="AS31" s="22" t="s">
+      <c r="AN31" s="20"/>
+      <c r="AO31" s="20"/>
+      <c r="AP31" s="20"/>
+      <c r="AQ31" s="20"/>
+      <c r="AR31" s="20"/>
+      <c r="AS31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="AT31" s="22"/>
-      <c r="AU31" s="22"/>
-      <c r="AV31" s="22"/>
-      <c r="AW31" s="22"/>
-      <c r="AX31" s="22"/>
-      <c r="AY31" s="22" t="s">
+      <c r="AT31" s="20"/>
+      <c r="AU31" s="20"/>
+      <c r="AV31" s="20"/>
+      <c r="AW31" s="20"/>
+      <c r="AX31" s="20"/>
+      <c r="AY31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="AZ31" s="22"/>
-      <c r="BA31" s="22"/>
-      <c r="BB31" s="22"/>
-      <c r="BC31" s="22"/>
-      <c r="BD31" s="22"/>
-      <c r="BE31" s="22" t="s">
+      <c r="AZ31" s="20"/>
+      <c r="BA31" s="20"/>
+      <c r="BB31" s="20"/>
+      <c r="BC31" s="20"/>
+      <c r="BD31" s="20"/>
+      <c r="BE31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="BF31" s="22"/>
-      <c r="BG31" s="22"/>
-      <c r="BH31" s="22"/>
-      <c r="BI31" s="22"/>
-      <c r="BJ31" s="22"/>
-      <c r="BK31" s="22" t="s">
+      <c r="BF31" s="20"/>
+      <c r="BG31" s="20"/>
+      <c r="BH31" s="20"/>
+      <c r="BI31" s="20"/>
+      <c r="BJ31" s="20"/>
+      <c r="BK31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="BL31" s="22"/>
-      <c r="BM31" s="22"/>
-      <c r="BN31" s="22"/>
-      <c r="BO31" s="22"/>
-      <c r="BP31" s="22"/>
-      <c r="BQ31" s="22" t="s">
+      <c r="BL31" s="20"/>
+      <c r="BM31" s="20"/>
+      <c r="BN31" s="20"/>
+      <c r="BO31" s="20"/>
+      <c r="BP31" s="20"/>
+      <c r="BQ31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="BR31" s="22"/>
-      <c r="BS31" s="22"/>
-      <c r="BT31" s="22"/>
-      <c r="BU31" s="22"/>
-      <c r="BV31" s="22"/>
-      <c r="BW31" s="22" t="s">
+      <c r="BR31" s="20"/>
+      <c r="BS31" s="20"/>
+      <c r="BT31" s="20"/>
+      <c r="BU31" s="20"/>
+      <c r="BV31" s="20"/>
+      <c r="BW31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="BX31" s="22"/>
-      <c r="BY31" s="22"/>
-      <c r="BZ31" s="22"/>
-      <c r="CA31" s="22"/>
-      <c r="CB31" s="22"/>
-      <c r="CC31" s="22" t="s">
+      <c r="BX31" s="20"/>
+      <c r="BY31" s="20"/>
+      <c r="BZ31" s="20"/>
+      <c r="CA31" s="20"/>
+      <c r="CB31" s="20"/>
+      <c r="CC31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="CD31" s="22"/>
-      <c r="CE31" s="22"/>
-      <c r="CF31" s="22"/>
-      <c r="CG31" s="22"/>
-      <c r="CH31" s="22"/>
-      <c r="CI31" s="22" t="s">
+      <c r="CD31" s="20"/>
+      <c r="CE31" s="20"/>
+      <c r="CF31" s="20"/>
+      <c r="CG31" s="20"/>
+      <c r="CH31" s="20"/>
+      <c r="CI31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="CJ31" s="22"/>
-      <c r="CK31" s="22"/>
-      <c r="CL31" s="22"/>
-      <c r="CM31" s="22"/>
-      <c r="CN31" s="22"/>
-    </row>
-    <row r="32" spans="1:96" x14ac:dyDescent="0.45">
-      <c r="AG32" s="22">
+      <c r="CJ31" s="20"/>
+      <c r="CK31" s="20"/>
+      <c r="CL31" s="20"/>
+      <c r="CM31" s="20"/>
+      <c r="CN31" s="20"/>
+    </row>
+    <row r="32" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="AG32" s="20">
         <v>25</v>
       </c>
-      <c r="AH32" s="22"/>
-      <c r="AI32" s="22"/>
-      <c r="AJ32" s="22"/>
-      <c r="AK32" s="22"/>
-      <c r="AL32" s="22"/>
-      <c r="AM32" s="22">
+      <c r="AH32" s="20"/>
+      <c r="AI32" s="20"/>
+      <c r="AJ32" s="20"/>
+      <c r="AK32" s="20"/>
+      <c r="AL32" s="20"/>
+      <c r="AM32" s="20">
         <v>25</v>
       </c>
-      <c r="AN32" s="22"/>
-      <c r="AO32" s="22"/>
-      <c r="AP32" s="22"/>
-      <c r="AQ32" s="22"/>
-      <c r="AR32" s="22"/>
-      <c r="AS32" s="22">
+      <c r="AN32" s="20"/>
+      <c r="AO32" s="20"/>
+      <c r="AP32" s="20"/>
+      <c r="AQ32" s="20"/>
+      <c r="AR32" s="20"/>
+      <c r="AS32" s="20">
         <v>25</v>
       </c>
-      <c r="AT32" s="22"/>
-      <c r="AU32" s="22"/>
-      <c r="AV32" s="22"/>
-      <c r="AW32" s="22"/>
-      <c r="AX32" s="22"/>
-      <c r="AY32" s="22">
+      <c r="AT32" s="20"/>
+      <c r="AU32" s="20"/>
+      <c r="AV32" s="20"/>
+      <c r="AW32" s="20"/>
+      <c r="AX32" s="20"/>
+      <c r="AY32" s="20">
         <v>25</v>
       </c>
-      <c r="AZ32" s="22"/>
-      <c r="BA32" s="22"/>
-      <c r="BB32" s="22"/>
-      <c r="BC32" s="22"/>
-      <c r="BD32" s="22"/>
-      <c r="BE32" s="22">
+      <c r="AZ32" s="20"/>
+      <c r="BA32" s="20"/>
+      <c r="BB32" s="20"/>
+      <c r="BC32" s="20"/>
+      <c r="BD32" s="20"/>
+      <c r="BE32" s="20">
         <v>26</v>
       </c>
-      <c r="BF32" s="22"/>
-      <c r="BG32" s="22"/>
-      <c r="BH32" s="22"/>
-      <c r="BI32" s="22"/>
-      <c r="BJ32" s="22"/>
-      <c r="BK32" s="22">
+      <c r="BF32" s="20"/>
+      <c r="BG32" s="20"/>
+      <c r="BH32" s="20"/>
+      <c r="BI32" s="20"/>
+      <c r="BJ32" s="20"/>
+      <c r="BK32" s="20">
         <v>26</v>
       </c>
-      <c r="BL32" s="22"/>
-      <c r="BM32" s="22"/>
-      <c r="BN32" s="22"/>
-      <c r="BO32" s="22"/>
-      <c r="BP32" s="22"/>
-      <c r="BQ32" s="22">
+      <c r="BL32" s="20"/>
+      <c r="BM32" s="20"/>
+      <c r="BN32" s="20"/>
+      <c r="BO32" s="20"/>
+      <c r="BP32" s="20"/>
+      <c r="BQ32" s="20">
         <v>26</v>
       </c>
-      <c r="BR32" s="22"/>
-      <c r="BS32" s="22"/>
-      <c r="BT32" s="22"/>
-      <c r="BU32" s="22"/>
-      <c r="BV32" s="22"/>
-      <c r="BW32" s="22">
+      <c r="BR32" s="20"/>
+      <c r="BS32" s="20"/>
+      <c r="BT32" s="20"/>
+      <c r="BU32" s="20"/>
+      <c r="BV32" s="20"/>
+      <c r="BW32" s="20">
         <v>26</v>
       </c>
-      <c r="BX32" s="22"/>
-      <c r="BY32" s="22"/>
-      <c r="BZ32" s="22"/>
-      <c r="CA32" s="22"/>
-      <c r="CB32" s="22"/>
-      <c r="CC32" s="22">
+      <c r="BX32" s="20"/>
+      <c r="BY32" s="20"/>
+      <c r="BZ32" s="20"/>
+      <c r="CA32" s="20"/>
+      <c r="CB32" s="20"/>
+      <c r="CC32" s="20">
         <v>26</v>
       </c>
-      <c r="CD32" s="22"/>
-      <c r="CE32" s="22"/>
-      <c r="CF32" s="22"/>
-      <c r="CG32" s="22"/>
-      <c r="CH32" s="22"/>
-      <c r="CI32" s="22">
+      <c r="CD32" s="20"/>
+      <c r="CE32" s="20"/>
+      <c r="CF32" s="20"/>
+      <c r="CG32" s="20"/>
+      <c r="CH32" s="20"/>
+      <c r="CI32" s="20">
         <v>26</v>
       </c>
-      <c r="CJ32" s="22"/>
-      <c r="CK32" s="22"/>
-      <c r="CL32" s="22"/>
-      <c r="CM32" s="22"/>
-      <c r="CN32" s="22"/>
+      <c r="CJ32" s="20"/>
+      <c r="CK32" s="20"/>
+      <c r="CL32" s="20"/>
+      <c r="CM32" s="20"/>
+      <c r="CN32" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="166">
-    <mergeCell ref="BK32:BP32"/>
-    <mergeCell ref="BQ32:BV32"/>
-    <mergeCell ref="BW32:CB32"/>
-    <mergeCell ref="CC32:CH32"/>
-    <mergeCell ref="CI32:CN32"/>
-    <mergeCell ref="AG32:AL32"/>
-    <mergeCell ref="AM32:AR32"/>
-    <mergeCell ref="AS32:AX32"/>
-    <mergeCell ref="AY32:BD32"/>
-    <mergeCell ref="BE32:BJ32"/>
-    <mergeCell ref="BK31:BP31"/>
-    <mergeCell ref="BQ31:BV31"/>
-    <mergeCell ref="BW31:CB31"/>
-    <mergeCell ref="CC31:CH31"/>
-    <mergeCell ref="CI31:CN31"/>
-    <mergeCell ref="AG31:AL31"/>
-    <mergeCell ref="AM31:AR31"/>
-    <mergeCell ref="AS31:AX31"/>
-    <mergeCell ref="AY31:BD31"/>
-    <mergeCell ref="BE31:BJ31"/>
-    <mergeCell ref="BK29:BP29"/>
-    <mergeCell ref="BQ29:BV29"/>
-    <mergeCell ref="BW29:CB29"/>
-    <mergeCell ref="CC29:CH29"/>
-    <mergeCell ref="CI29:CN29"/>
-    <mergeCell ref="AG29:AL29"/>
-    <mergeCell ref="AM29:AR29"/>
-    <mergeCell ref="AS29:AX29"/>
-    <mergeCell ref="AY29:BD29"/>
-    <mergeCell ref="BE29:BJ29"/>
-    <mergeCell ref="BK28:BP28"/>
-    <mergeCell ref="BQ28:BV28"/>
-    <mergeCell ref="BW28:CB28"/>
-    <mergeCell ref="CC28:CH28"/>
-    <mergeCell ref="CI28:CN28"/>
-    <mergeCell ref="AG28:AL28"/>
-    <mergeCell ref="AM28:AR28"/>
-    <mergeCell ref="AS28:AX28"/>
-    <mergeCell ref="AY28:BD28"/>
-    <mergeCell ref="BE28:BJ28"/>
-    <mergeCell ref="BU24:CB24"/>
-    <mergeCell ref="CC24:CJ24"/>
-    <mergeCell ref="CK24:CR24"/>
-    <mergeCell ref="AG26:AN26"/>
-    <mergeCell ref="AO26:AV26"/>
-    <mergeCell ref="AW26:BD26"/>
-    <mergeCell ref="BE26:BL26"/>
-    <mergeCell ref="BM26:BT26"/>
-    <mergeCell ref="BU26:CB26"/>
-    <mergeCell ref="CC26:CJ26"/>
-    <mergeCell ref="CK26:CR26"/>
-    <mergeCell ref="AG24:AN24"/>
-    <mergeCell ref="AO24:AV24"/>
-    <mergeCell ref="AW24:BD24"/>
-    <mergeCell ref="BE24:BL24"/>
-    <mergeCell ref="BM24:BT24"/>
-    <mergeCell ref="Y28:AC28"/>
-    <mergeCell ref="AD28:AF28"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="I29:M29"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="Q29:S29"/>
-    <mergeCell ref="T29:X29"/>
-    <mergeCell ref="Y29:AC29"/>
-    <mergeCell ref="AD29:AF29"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="I28:M28"/>
-    <mergeCell ref="N28:P28"/>
-    <mergeCell ref="Q28:S28"/>
-    <mergeCell ref="T28:X28"/>
-    <mergeCell ref="Y26:AC26"/>
-    <mergeCell ref="AD26:AF26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="I27:M27"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="Q27:S27"/>
-    <mergeCell ref="T27:X27"/>
-    <mergeCell ref="Y27:AC27"/>
-    <mergeCell ref="AD27:AF27"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="I26:M26"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="Q26:S26"/>
-    <mergeCell ref="T26:X26"/>
+    <mergeCell ref="Y19:AC19"/>
+    <mergeCell ref="AD19:AF19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="I20:M20"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="T20:X20"/>
+    <mergeCell ref="Y20:AC20"/>
+    <mergeCell ref="AD20:AF20"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="I19:M19"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="T19:X19"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="I15:P15"/>
+    <mergeCell ref="Q15:X15"/>
+    <mergeCell ref="Y15:AF15"/>
+    <mergeCell ref="A14:AF14"/>
+    <mergeCell ref="Y17:AC17"/>
+    <mergeCell ref="AD17:AF17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="I18:M18"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="T18:X18"/>
+    <mergeCell ref="Y18:AC18"/>
+    <mergeCell ref="AD18:AF18"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="I17:M17"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="T17:X17"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="I10:M10"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="AD10:AF10"/>
+    <mergeCell ref="Y10:AC10"/>
+    <mergeCell ref="T10:X10"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="AD11:AF11"/>
+    <mergeCell ref="Y11:AC11"/>
+    <mergeCell ref="T11:X11"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="Q6:X6"/>
+    <mergeCell ref="Y6:AF6"/>
+    <mergeCell ref="AD9:AF9"/>
+    <mergeCell ref="AD8:AF8"/>
+    <mergeCell ref="Y9:AC9"/>
+    <mergeCell ref="Y8:AC8"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="T8:X8"/>
+    <mergeCell ref="T9:X9"/>
     <mergeCell ref="A23:AF23"/>
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="I24:P24"/>
@@ -7410,64 +7390,90 @@
     <mergeCell ref="I8:M8"/>
     <mergeCell ref="N8:P8"/>
     <mergeCell ref="I9:M9"/>
-    <mergeCell ref="Q6:X6"/>
-    <mergeCell ref="Y6:AF6"/>
-    <mergeCell ref="AD9:AF9"/>
-    <mergeCell ref="AD8:AF8"/>
-    <mergeCell ref="Y9:AC9"/>
-    <mergeCell ref="Y8:AC8"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="T8:X8"/>
-    <mergeCell ref="T9:X9"/>
-    <mergeCell ref="I11:M11"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="I10:M10"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="AD10:AF10"/>
-    <mergeCell ref="Y10:AC10"/>
-    <mergeCell ref="T10:X10"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="AD11:AF11"/>
-    <mergeCell ref="Y11:AC11"/>
-    <mergeCell ref="T11:X11"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="I15:P15"/>
-    <mergeCell ref="Q15:X15"/>
-    <mergeCell ref="Y15:AF15"/>
-    <mergeCell ref="A14:AF14"/>
-    <mergeCell ref="Y17:AC17"/>
-    <mergeCell ref="AD17:AF17"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="I18:M18"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="T18:X18"/>
-    <mergeCell ref="Y18:AC18"/>
-    <mergeCell ref="AD18:AF18"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="I17:M17"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="T17:X17"/>
-    <mergeCell ref="Y19:AC19"/>
-    <mergeCell ref="AD19:AF19"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="I20:M20"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="T20:X20"/>
-    <mergeCell ref="Y20:AC20"/>
-    <mergeCell ref="AD20:AF20"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="I19:M19"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="T19:X19"/>
+    <mergeCell ref="Y26:AC26"/>
+    <mergeCell ref="AD26:AF26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="I27:M27"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="Q27:S27"/>
+    <mergeCell ref="T27:X27"/>
+    <mergeCell ref="Y27:AC27"/>
+    <mergeCell ref="AD27:AF27"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="I26:M26"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="Q26:S26"/>
+    <mergeCell ref="T26:X26"/>
+    <mergeCell ref="Y28:AC28"/>
+    <mergeCell ref="AD28:AF28"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="I29:M29"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="Q29:S29"/>
+    <mergeCell ref="T29:X29"/>
+    <mergeCell ref="Y29:AC29"/>
+    <mergeCell ref="AD29:AF29"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="I28:M28"/>
+    <mergeCell ref="N28:P28"/>
+    <mergeCell ref="Q28:S28"/>
+    <mergeCell ref="T28:X28"/>
+    <mergeCell ref="BU24:CB24"/>
+    <mergeCell ref="CC24:CJ24"/>
+    <mergeCell ref="CK24:CR24"/>
+    <mergeCell ref="AG26:AN26"/>
+    <mergeCell ref="AO26:AV26"/>
+    <mergeCell ref="AW26:BD26"/>
+    <mergeCell ref="BE26:BL26"/>
+    <mergeCell ref="BM26:BT26"/>
+    <mergeCell ref="BU26:CB26"/>
+    <mergeCell ref="CC26:CJ26"/>
+    <mergeCell ref="CK26:CR26"/>
+    <mergeCell ref="AG24:AN24"/>
+    <mergeCell ref="AO24:AV24"/>
+    <mergeCell ref="AW24:BD24"/>
+    <mergeCell ref="BE24:BL24"/>
+    <mergeCell ref="BM24:BT24"/>
+    <mergeCell ref="BK28:BP28"/>
+    <mergeCell ref="BQ28:BV28"/>
+    <mergeCell ref="BW28:CB28"/>
+    <mergeCell ref="CC28:CH28"/>
+    <mergeCell ref="CI28:CN28"/>
+    <mergeCell ref="AG28:AL28"/>
+    <mergeCell ref="AM28:AR28"/>
+    <mergeCell ref="AS28:AX28"/>
+    <mergeCell ref="AY28:BD28"/>
+    <mergeCell ref="BE28:BJ28"/>
+    <mergeCell ref="BK29:BP29"/>
+    <mergeCell ref="BQ29:BV29"/>
+    <mergeCell ref="BW29:CB29"/>
+    <mergeCell ref="CC29:CH29"/>
+    <mergeCell ref="CI29:CN29"/>
+    <mergeCell ref="AG29:AL29"/>
+    <mergeCell ref="AM29:AR29"/>
+    <mergeCell ref="AS29:AX29"/>
+    <mergeCell ref="AY29:BD29"/>
+    <mergeCell ref="BE29:BJ29"/>
+    <mergeCell ref="BK31:BP31"/>
+    <mergeCell ref="BQ31:BV31"/>
+    <mergeCell ref="BW31:CB31"/>
+    <mergeCell ref="CC31:CH31"/>
+    <mergeCell ref="CI31:CN31"/>
+    <mergeCell ref="AG31:AL31"/>
+    <mergeCell ref="AM31:AR31"/>
+    <mergeCell ref="AS31:AX31"/>
+    <mergeCell ref="AY31:BD31"/>
+    <mergeCell ref="BE31:BJ31"/>
+    <mergeCell ref="BK32:BP32"/>
+    <mergeCell ref="BQ32:BV32"/>
+    <mergeCell ref="BW32:CB32"/>
+    <mergeCell ref="CC32:CH32"/>
+    <mergeCell ref="CI32:CN32"/>
+    <mergeCell ref="AG32:AL32"/>
+    <mergeCell ref="AM32:AR32"/>
+    <mergeCell ref="AS32:AX32"/>
+    <mergeCell ref="AY32:BD32"/>
+    <mergeCell ref="BE32:BJ32"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -7482,30 +7488,30 @@
       <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.86328125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="4.796875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="8.46484375" style="7" customWidth="1"/>
-    <col min="4" max="9" width="5.53125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="11.53125" style="7"/>
-    <col min="11" max="11" width="4.796875" style="7" customWidth="1"/>
-    <col min="12" max="12" width="8.46484375" style="7" customWidth="1"/>
-    <col min="13" max="18" width="5.53125" style="7" customWidth="1"/>
-    <col min="19" max="16384" width="11.53125" style="7"/>
+    <col min="1" max="1" width="5.88671875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="4.77734375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" style="7" customWidth="1"/>
+    <col min="4" max="9" width="5.5546875" style="7" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" style="7"/>
+    <col min="11" max="11" width="4.77734375" style="7" customWidth="1"/>
+    <col min="12" max="12" width="8.44140625" style="7" customWidth="1"/>
+    <col min="13" max="18" width="5.5546875" style="7" customWidth="1"/>
+    <col min="19" max="16384" width="11.5546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B1" s="20" t="s">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B1" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
       <c r="E1" s="7">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3" s="36" t="s">
         <v>43</v>
       </c>
@@ -7531,7 +7537,7 @@
       <c r="Q3" s="36"/>
       <c r="R3" s="36"/>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
       <c r="D4" s="11">
@@ -7573,7 +7579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="37" t="s">
         <v>41</v>
       </c>
@@ -7635,7 +7641,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="37"/>
       <c r="C6" s="11">
         <v>0.02</v>
@@ -7693,7 +7699,7 @@
         <v>4.0000000000000003E-5</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" s="37"/>
       <c r="C7" s="11">
         <v>0.03</v>
@@ -7751,7 +7757,7 @@
         <v>8.9999999999999992E-5</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="37"/>
       <c r="C8" s="11">
         <v>0.05</v>
@@ -7809,7 +7815,7 @@
         <v>2.5000000000000001E-4</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="37"/>
       <c r="C9" s="11">
         <v>0.1</v>
@@ -7867,7 +7873,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" s="37"/>
       <c r="C10" s="11">
         <v>0.2</v>
@@ -7925,7 +7931,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11" s="37"/>
       <c r="C11" s="11">
         <v>0.3</v>
@@ -7983,7 +7989,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B12" s="37"/>
       <c r="C12" s="11">
         <v>0.5</v>
@@ -8041,7 +8047,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B13" s="37"/>
       <c r="C13" s="11">
         <v>1</v>
@@ -8127,14 +8133,14 @@
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>4.2</v>
       </c>
@@ -8142,7 +8148,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>4.0999999999999996</v>
       </c>
@@ -8150,7 +8156,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -8158,7 +8164,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3.9</v>
       </c>
@@ -8166,7 +8172,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3.8</v>
       </c>
@@ -8174,7 +8180,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3.7</v>
       </c>
@@ -8182,7 +8188,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3.6</v>
       </c>
@@ -8190,7 +8196,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3.5</v>
       </c>
@@ -8198,7 +8204,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3.4</v>
       </c>
@@ -8206,7 +8212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3.3</v>
       </c>
@@ -8214,7 +8220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3.19999999999999</v>
       </c>
@@ -8222,7 +8228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3.0999999999999899</v>
       </c>
@@ -8230,7 +8236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>115</v>
       </c>
@@ -8247,7 +8253,7 @@
         <v>-35946.107099583001</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="16">
         <v>4.2</v>
       </c>
@@ -8265,7 +8271,7 @@
         <v>52310.9370900473</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="16">
         <v>4.1500000000000004</v>
       </c>
@@ -8283,7 +8289,7 @@
         <v>-29962.807104122399</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="16">
         <v>4.0999999999999996</v>
       </c>
@@ -8301,7 +8307,7 @@
         <v>8431.4105127834991</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="16">
         <v>4.05</v>
       </c>
@@ -8319,7 +8325,7 @@
         <v>-1164.3507315616</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="16">
         <v>4</v>
       </c>
@@ -8337,7 +8343,7 @@
         <v>63.147575745899999</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="16">
         <v>3.95</v>
       </c>
@@ -8349,7 +8355,7 @@
         <v>88.405632938047347</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="16">
         <v>3.9</v>
       </c>
@@ -8361,7 +8367,7 @@
         <v>83.814032900780148</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="16">
         <v>3.85</v>
       </c>
@@ -8373,7 +8379,7 @@
         <v>78.646063650106953</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="16">
         <v>3.8</v>
       </c>
@@ -8385,7 +8391,7 @@
         <v>73.001946173659235</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="16">
         <v>3.75</v>
       </c>
@@ -8397,7 +8403,7 @@
         <v>66.989587474461587</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="16">
         <v>3.7</v>
       </c>
@@ -8409,7 +8415,7 @@
         <v>60.722212536311417</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="16">
         <v>3.65</v>
       </c>
@@ -8421,7 +8427,7 @@
         <v>54.315996290177281</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="16">
         <v>3.6</v>
       </c>
@@ -8433,7 +8439,7 @@
         <v>47.887695580277068</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="16">
         <v>3.55</v>
       </c>
@@ -8445,7 +8451,7 @@
         <v>41.55228112925397</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="16">
         <v>3.5</v>
       </c>
@@ -8457,7 +8463,7 @@
         <v>35.420569505040476</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="16">
         <v>3.45</v>
       </c>
@@ -8469,7 +8475,7 @@
         <v>29.596855085597781</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="16">
         <v>3.4</v>
       </c>
@@ -8481,7 +8487,7 @@
         <v>24.176542026129027</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="16">
         <v>3.35</v>
       </c>
@@ -8493,7 +8499,7 @@
         <v>19.243776223993336</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="16">
         <v>3.3</v>
       </c>
@@ -8505,7 +8511,7 @@
         <v>14.869077284987725</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="16">
         <v>3.25</v>
       </c>
@@ -8517,7 +8523,7 @@
         <v>11.106970489425294</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="16">
         <v>3.2</v>
       </c>
@@ -8529,7 +8535,7 @@
         <v>7.9936187574858195</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="16">
         <v>3.15</v>
       </c>
@@ -8541,7 +8547,7 @@
         <v>5.5444546161379549</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="16">
         <v>3.1</v>
       </c>
@@ -8553,7 +8559,7 @@
         <v>3.7518121635876014</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="16">
         <v>3.05</v>
       </c>
@@ -8565,7 +8571,7 @@
         <v>2.5825590366948745</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="16">
         <v>3</v>
       </c>
@@ -8577,7 +8583,7 @@
         <v>1.9757283759172424</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="16">
         <v>2.95</v>
       </c>
@@ -8586,7 +8592,7 @@
       </c>
       <c r="C56" s="16"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="16">
         <v>2.9</v>
       </c>
@@ -8595,7 +8601,7 @@
       </c>
       <c r="C57" s="16"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="16">
         <v>2.85</v>
       </c>
@@ -8604,7 +8610,7 @@
       </c>
       <c r="C58" s="16"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="16">
         <v>2.8</v>
       </c>
@@ -8613,7 +8619,7 @@
       </c>
       <c r="C59" s="16"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="16">
         <v>2.7500000000000102</v>
       </c>
@@ -8622,7 +8628,7 @@
       </c>
       <c r="C60" s="16"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="16">
         <v>2.7000000000000099</v>
       </c>
@@ -8631,7 +8637,7 @@
       </c>
       <c r="C61" s="16"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="16">
         <v>2.6500000000000101</v>
       </c>
@@ -8640,7 +8646,7 @@
       </c>
       <c r="C62" s="16"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="16">
         <v>2.6000000000000099</v>
       </c>
@@ -8663,12 +8669,12 @@
       <selection activeCell="I6" sqref="I6:S11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="19" width="4.19921875" customWidth="1"/>
+    <col min="1" max="19" width="4.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
         <v>21</v>
       </c>
@@ -8691,7 +8697,7 @@
       <c r="R1" s="7"/>
       <c r="S1" s="7"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>7</v>
       </c>
@@ -8744,34 +8750,34 @@
       <c r="R2" s="7"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="32" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="32" t="s">
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="33"/>
-      <c r="P3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="35"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -8792,7 +8798,7 @@
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -8813,7 +8819,7 @@
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -8833,12 +8839,12 @@
       <c r="O6" s="25"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="20" t="s">
+      <c r="R6" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="S6" s="20"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="S6" s="22"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -8879,7 +8885,7 @@
       </c>
       <c r="S7" s="38"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -8888,23 +8894,23 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20" t="s">
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -8913,23 +8919,23 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="20">
+      <c r="I9" s="22">
         <v>17</v>
       </c>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20">
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22">
         <v>4</v>
       </c>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -8943,16 +8949,16 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
-      <c r="N10" s="20" t="s">
+      <c r="N10" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -8966,24 +8972,18 @@
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
-      <c r="N11" s="21">
+      <c r="N11" s="23">
         <f>100/(2^3-1)*N9</f>
         <v>57.142857142857146</v>
       </c>
-      <c r="O11" s="21"/>
-      <c r="P11" s="21"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="I3:M3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="I6:P6"/>
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="R7:S7"/>
     <mergeCell ref="I8:M8"/>
@@ -8991,6 +8991,12 @@
     <mergeCell ref="I9:M9"/>
     <mergeCell ref="N9:P9"/>
     <mergeCell ref="N10:P10"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="I6:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>